<commit_message>
delujoc program z zamenjavo
</commit_message>
<xml_diff>
--- a/data/AHLdelegacije.xlsx
+++ b/data/AHLdelegacije.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet sheetId="1" name="AHL" state="visible" r:id="rId4"/>
     <sheet sheetId="2" name="EBEL" state="visible" r:id="rId5"/>
     <sheet sheetId="3" name="AHL_DAT" state="visible" r:id="rId6"/>
+    <sheet sheetId="4" name="AHL_DAT_STRING" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="162">
   <si>
     <t>slo</t>
   </si>
@@ -435,7 +436,73 @@
     <t>2019-11-19</t>
   </si>
   <si>
+    <t>2019-11-07</t>
+  </si>
+  <si>
+    <t>2019-11-09</t>
+  </si>
+  <si>
     <t>HLAVATY</t>
+  </si>
+  <si>
+    <t>Eishalle Dornbirn;GAMPER;HOLZER;MARTIN;SPIEGEL</t>
+  </si>
+  <si>
+    <t>Hala Tivoli Ljubljana;KUMMER;WIDMANN;PUFF;SCHWEIGHOFER</t>
+  </si>
+  <si>
+    <t>Eishalle Wien-Kagran;HLAVATY;SUPPER;RIECKEN;WEISS</t>
+  </si>
+  <si>
+    <t>Eishalle Wien Kagran;REISINGER;SUPPER;KAINBERGER;WIMMLER</t>
+  </si>
+  <si>
+    <t>Feldkirch Vorarlberghalle;BERNEKER;STOLC;MARTIN;SPIEGEL</t>
+  </si>
+  <si>
+    <t>Feldkirch Vorarlberghalle;RUETZ;SCHAUER;RINKER;TSCHREPITSCH</t>
+  </si>
+  <si>
+    <t>Eissporthalle Linz;LENDL;LOICHT;LEGAT;SCHONAKLENER</t>
+  </si>
+  <si>
+    <t>Ledena dvorana Podmežakla;DURCHNER;LESNIAK;MARCHARDT;SCHWEIGHOFER</t>
+  </si>
+  <si>
+    <t>Eisarena Salzburg;LAZZERI;OREL;MATTHEY;MOIDL</t>
+  </si>
+  <si>
+    <t>Eishalle Zell am See;KUMMER;PODLESNIK;HOLZER;PUFF</t>
+  </si>
+  <si>
+    <t>Kitzbühel Sportpark;BAJT;PODLESNIK;BERGANT;HUBER</t>
+  </si>
+  <si>
+    <t>Pranives Wolkenstein;BENVEGNU;GIACOMOZZI;BEDANA;RIGONI</t>
+  </si>
+  <si>
+    <t>Rienzstadion Bruneck;STEFENELLI;VIRTA;MANTOVANI;SLAVIERO</t>
+  </si>
+  <si>
+    <t>KeineSorgenEisarena;RUETZ;WIDMANN;MATTHEY;MOIDL</t>
+  </si>
+  <si>
+    <t>Arena Ritten;LEGA;RUETZ;BASSO;PESEK</t>
+  </si>
+  <si>
+    <t>Kitzbühel Sportpark;GAMPER;MOSCHEN;MARTIN;PACE</t>
+  </si>
+  <si>
+    <t>Stadio Olympico;MOSCHEN;PINIE;DE ZORDO;PIRAS</t>
+  </si>
+  <si>
+    <t>Feldkirch Vorarlberghalle;HOLZER;LEGA;TERRAGNI;VIGNOLO</t>
+  </si>
+  <si>
+    <t>Dornbirn Messestadion;BULOVEC;SCHAUER;HUBER;RINKER</t>
+  </si>
+  <si>
+    <t>Weihenstephan Arena;PINIE;STEFENELLI;DE ZORDO;PIRAS</t>
   </si>
 </sst>
 </file>
@@ -788,82 +855,82 @@
       <selection activeCell="BT10" sqref="BT10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="14.45" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" customWidth="1"/>
-    <col min="7" max="7" width="15.5546875" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" customWidth="1"/>
-    <col min="12" max="12" width="12.5546875" customWidth="1"/>
-    <col min="13" max="13" width="11.44140625" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" customWidth="1"/>
-    <col min="15" max="15" width="11.6640625" customWidth="1"/>
-    <col min="16" max="16" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" customWidth="1"/>
+    <col min="16" max="16" width="17.28515625" customWidth="1"/>
     <col min="17" max="17" width="16" customWidth="1"/>
-    <col min="18" max="18" width="14.44140625" customWidth="1"/>
-    <col min="19" max="19" width="12.5546875" customWidth="1"/>
-    <col min="20" max="20" width="14.5546875" customWidth="1"/>
+    <col min="18" max="18" width="14.42578125" customWidth="1"/>
+    <col min="19" max="19" width="12.5703125" customWidth="1"/>
+    <col min="20" max="20" width="14.5703125" customWidth="1"/>
     <col min="21" max="21" width="10" customWidth="1"/>
-    <col min="22" max="22" width="10.109375" customWidth="1"/>
-    <col min="23" max="23" width="11.109375" customWidth="1"/>
-    <col min="24" max="24" width="10.6640625" customWidth="1"/>
-    <col min="25" max="25" width="12.88671875" customWidth="1"/>
-    <col min="26" max="26" width="13.33203125" customWidth="1"/>
-    <col min="27" max="27" width="11.88671875" customWidth="1"/>
-    <col min="28" max="28" width="11.44140625" customWidth="1"/>
-    <col min="29" max="29" width="11.33203125" customWidth="1"/>
-    <col min="30" max="30" width="11.109375" customWidth="1"/>
+    <col min="22" max="22" width="10.140625" customWidth="1"/>
+    <col min="23" max="23" width="11.140625" customWidth="1"/>
+    <col min="24" max="24" width="10.7109375" customWidth="1"/>
+    <col min="25" max="25" width="12.85546875" customWidth="1"/>
+    <col min="26" max="26" width="13.28515625" customWidth="1"/>
+    <col min="27" max="27" width="11.85546875" customWidth="1"/>
+    <col min="28" max="28" width="11.42578125" customWidth="1"/>
+    <col min="29" max="29" width="11.28515625" customWidth="1"/>
+    <col min="30" max="30" width="11.140625" customWidth="1"/>
     <col min="31" max="32" width="11" customWidth="1"/>
-    <col min="33" max="33" width="10.109375" customWidth="1"/>
-    <col min="34" max="34" width="13.33203125" customWidth="1"/>
-    <col min="35" max="35" width="11.88671875" customWidth="1"/>
-    <col min="36" max="36" width="11.6640625" customWidth="1"/>
-    <col min="37" max="37" width="10.44140625" customWidth="1"/>
-    <col min="38" max="38" width="12.109375" customWidth="1"/>
-    <col min="39" max="39" width="10.88671875" customWidth="1"/>
-    <col min="40" max="40" width="13.5546875" customWidth="1"/>
-    <col min="41" max="41" width="10.109375" customWidth="1"/>
-    <col min="42" max="42" width="11.33203125" customWidth="1"/>
-    <col min="43" max="43" width="11.109375" customWidth="1"/>
-    <col min="44" max="44" width="10.6640625" customWidth="1"/>
+    <col min="33" max="33" width="10.140625" customWidth="1"/>
+    <col min="34" max="34" width="13.28515625" customWidth="1"/>
+    <col min="35" max="35" width="11.85546875" customWidth="1"/>
+    <col min="36" max="36" width="11.7109375" customWidth="1"/>
+    <col min="37" max="37" width="10.42578125" customWidth="1"/>
+    <col min="38" max="38" width="12.140625" customWidth="1"/>
+    <col min="39" max="39" width="10.85546875" customWidth="1"/>
+    <col min="40" max="40" width="13.5703125" customWidth="1"/>
+    <col min="41" max="41" width="10.140625" customWidth="1"/>
+    <col min="42" max="42" width="11.28515625" customWidth="1"/>
+    <col min="43" max="43" width="11.140625" customWidth="1"/>
+    <col min="44" max="44" width="10.7109375" customWidth="1"/>
     <col min="45" max="45" width="12" customWidth="1"/>
-    <col min="46" max="46" width="11.44140625" customWidth="1"/>
-    <col min="47" max="47" width="14.44140625" customWidth="1"/>
+    <col min="46" max="46" width="11.42578125" customWidth="1"/>
+    <col min="47" max="47" width="14.42578125" customWidth="1"/>
     <col min="48" max="48" width="12" customWidth="1"/>
-    <col min="49" max="49" width="10.109375" customWidth="1"/>
-    <col min="51" max="51" width="10.5546875" customWidth="1"/>
+    <col min="49" max="49" width="10.140625" customWidth="1"/>
+    <col min="51" max="51" width="10.5703125" customWidth="1"/>
     <col min="52" max="52" width="13" customWidth="1"/>
-    <col min="53" max="53" width="10.5546875" customWidth="1"/>
-    <col min="54" max="54" width="11.6640625" customWidth="1"/>
-    <col min="55" max="55" width="14.33203125" customWidth="1"/>
-    <col min="56" max="56" width="16.88671875" customWidth="1"/>
-    <col min="57" max="57" width="12.6640625" customWidth="1"/>
-    <col min="58" max="58" width="13.44140625" customWidth="1"/>
-    <col min="59" max="60" width="10.33203125" customWidth="1"/>
-    <col min="61" max="61" width="12.109375" customWidth="1"/>
+    <col min="53" max="53" width="10.5703125" customWidth="1"/>
+    <col min="54" max="54" width="11.7109375" customWidth="1"/>
+    <col min="55" max="55" width="14.28515625" customWidth="1"/>
+    <col min="56" max="56" width="16.85546875" customWidth="1"/>
+    <col min="57" max="57" width="12.7109375" customWidth="1"/>
+    <col min="58" max="58" width="13.42578125" customWidth="1"/>
+    <col min="59" max="60" width="10.28515625" customWidth="1"/>
+    <col min="61" max="61" width="12.140625" customWidth="1"/>
     <col min="63" max="63" width="12" customWidth="1"/>
-    <col min="66" max="66" width="11.6640625" customWidth="1"/>
+    <col min="66" max="66" width="11.7109375" customWidth="1"/>
     <col min="67" max="67" width="23" customWidth="1"/>
-    <col min="68" max="68" width="11.44140625" customWidth="1"/>
-    <col min="69" max="69" width="12.5546875" customWidth="1"/>
-    <col min="70" max="70" width="10.33203125" customWidth="1"/>
-    <col min="72" max="72" width="15.109375" customWidth="1"/>
-    <col min="73" max="73" width="11.33203125" customWidth="1"/>
-    <col min="76" max="76" width="10.5546875" customWidth="1"/>
+    <col min="68" max="68" width="11.42578125" customWidth="1"/>
+    <col min="69" max="69" width="12.5703125" customWidth="1"/>
+    <col min="70" max="70" width="10.28515625" customWidth="1"/>
+    <col min="72" max="72" width="15.140625" customWidth="1"/>
+    <col min="73" max="73" width="11.28515625" customWidth="1"/>
+    <col min="76" max="76" width="10.5703125" customWidth="1"/>
     <col min="77" max="77" width="11" customWidth="1"/>
-    <col min="78" max="78" width="11.6640625" customWidth="1"/>
-    <col min="80" max="80" width="12.5546875" customWidth="1"/>
-    <col min="81" max="81" width="10.109375" customWidth="1"/>
+    <col min="78" max="78" width="11.7109375" customWidth="1"/>
+    <col min="80" max="80" width="12.5703125" customWidth="1"/>
+    <col min="81" max="81" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.4" customHeight="1" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="1" ht="14.45" customHeight="1" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1072,7 +1139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="14.4" customHeight="1" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="2" ht="14.45" customHeight="1" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>COUNTA(A4:A50)</f>
         <v>9</v>
@@ -1394,7 +1461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" ht="14.4" customHeight="1" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="3" ht="14.45" customHeight="1" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1636,7 +1703,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" ht="14.4" customHeight="1" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="4" ht="14.45" customHeight="1" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>43752</v>
       </c>
@@ -1879,7 +1946,7 @@
       </c>
       <c r="CC4" s="5"/>
     </row>
-    <row r="5" ht="14.4" customHeight="1" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="5" ht="14.45" customHeight="1" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>43759</v>
       </c>
@@ -2092,7 +2159,7 @@
       </c>
       <c r="CC5" s="5"/>
     </row>
-    <row r="6" ht="14.4" customHeight="1" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="6" ht="14.45" customHeight="1" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>43741</v>
       </c>
@@ -2286,7 +2353,7 @@
         <v>43741</v>
       </c>
     </row>
-    <row r="7" ht="14.4" customHeight="1" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="7" ht="14.45" customHeight="1" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -2474,7 +2541,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" ht="14.4" customHeight="1" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="8" ht="14.45" customHeight="1" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -2638,7 +2705,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" ht="14.4" customHeight="1" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="9" ht="14.45" customHeight="1" spans="1:72" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>91</v>
       </c>
@@ -2760,7 +2827,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" ht="14.4" customHeight="1" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="10" ht="14.45" customHeight="1" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>88</v>
       </c>
@@ -2852,7 +2919,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" ht="14.4" customHeight="1" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="11" ht="14.45" customHeight="1" spans="1:66" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>90</v>
       </c>
@@ -2911,7 +2978,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" ht="14.4" customHeight="1" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="12" ht="14.45" customHeight="1" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>84</v>
       </c>
@@ -2946,7 +3013,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" ht="14.4" customHeight="1" spans="14:52" x14ac:dyDescent="0.25">
+    <row r="13" ht="14.45" customHeight="1" spans="14:52" x14ac:dyDescent="0.25">
       <c r="N13" t="s">
         <v>90</v>
       </c>
@@ -2960,13 +3027,13 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" ht="14.4" customHeight="1" spans="6:52" x14ac:dyDescent="0.25">
+    <row r="14" ht="14.45" customHeight="1" spans="6:52" x14ac:dyDescent="0.25">
       <c r="F14" s="5"/>
       <c r="AZ14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="15" ht="14.4" customHeight="1" spans="52:52" x14ac:dyDescent="0.25">
+    <row r="15" ht="14.45" customHeight="1" spans="52:52" x14ac:dyDescent="0.25">
       <c r="AZ15" t="s">
         <v>84</v>
       </c>
@@ -2985,13 +3052,13 @@
       <selection activeCell="AK24" sqref="AK24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="14.45" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" customHeight="1"/>
   <cols>
-    <col min="30" max="30" width="17.109375" customWidth="1"/>
-    <col min="37" max="37" width="20.109375" customWidth="1"/>
+    <col min="30" max="30" width="17.140625" customWidth="1"/>
+    <col min="37" max="37" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="14.4" customHeight="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" ht="14.45" customHeight="1" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -3134,7 +3201,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="4" ht="14.4" customHeight="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" ht="14.45" customHeight="1" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>130</v>
       </c>
@@ -3277,7 +3344,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="5" ht="14.4" customHeight="1" spans="2:47" x14ac:dyDescent="0.25">
+    <row r="5" ht="14.45" customHeight="1" spans="2:47" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>135</v>
       </c>
@@ -3393,7 +3460,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" ht="14.4" customHeight="1" spans="2:45" x14ac:dyDescent="0.25">
+    <row r="6" ht="14.45" customHeight="1" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>95</v>
       </c>
@@ -3488,7 +3555,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" ht="14.4" customHeight="1" spans="2:45" x14ac:dyDescent="0.25">
+    <row r="7" ht="14.45" customHeight="1" spans="2:45" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>94</v>
       </c>
@@ -3562,7 +3629,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" ht="14.4" customHeight="1" spans="2:36" x14ac:dyDescent="0.25">
+    <row r="8" ht="14.45" customHeight="1" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>134</v>
       </c>
@@ -3600,7 +3667,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="9" ht="14.4" customHeight="1" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="9" ht="14.45" customHeight="1" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>130</v>
       </c>
@@ -3623,7 +3690,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" ht="14.4" customHeight="1" spans="7:34" x14ac:dyDescent="0.25">
+    <row r="10" ht="14.45" customHeight="1" spans="7:34" x14ac:dyDescent="0.25">
       <c r="G10" t="s">
         <v>130</v>
       </c>
@@ -3634,7 +3701,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="11" ht="14.4" customHeight="1" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="11" ht="14.45" customHeight="1" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M11" t="s">
         <v>134</v>
       </c>
@@ -3646,28 +3713,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:N42"/>
+  <dimension ref="A3:P42"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.3" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="14.45" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" customWidth="1"/>
-    <col min="7" max="7" width="14.5546875" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" customWidth="1"/>
+    <col min="1" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" customWidth="1"/>
     <col min="10" max="11" width="12" customWidth="1"/>
     <col min="12" max="12" width="11" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" customWidth="1"/>
+    <col min="14" max="15" width="16" customWidth="1"/>
+    <col min="16" max="16" width="13" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="14.4" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" ht="14.45" customHeight="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>84</v>
       </c>
@@ -3710,8 +3781,14 @@
       <c r="N3" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="4" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="O3" t="s">
+        <v>139</v>
+      </c>
+      <c r="P3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>30</v>
       </c>
@@ -3743,13 +3820,19 @@
         <v>15</v>
       </c>
       <c r="M4" t="s">
-        <v>59</v>
+        <v>141</v>
       </c>
       <c r="N4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="O4" t="s">
+        <v>53</v>
+      </c>
+      <c r="P4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>43</v>
       </c>
@@ -3781,13 +3864,19 @@
         <v>16</v>
       </c>
       <c r="M5" t="s">
-        <v>139</v>
+        <v>8</v>
       </c>
       <c r="N5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="O5" t="s">
+        <v>99</v>
+      </c>
+      <c r="P5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>40</v>
       </c>
@@ -3816,16 +3905,22 @@
         <v>37</v>
       </c>
       <c r="L6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="M6" t="s">
         <v>10</v>
       </c>
       <c r="N6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="O6" t="s">
+        <v>37</v>
+      </c>
+      <c r="P6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>6</v>
       </c>
@@ -3854,16 +3949,22 @@
         <v>77</v>
       </c>
       <c r="L7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M7" t="s">
         <v>33</v>
       </c>
       <c r="N7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="O7" t="s">
+        <v>77</v>
+      </c>
+      <c r="P7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>42</v>
       </c>
@@ -3885,17 +3986,14 @@
       <c r="J8" t="s">
         <v>64</v>
       </c>
-      <c r="K8" t="s">
-        <v>55</v>
-      </c>
       <c r="L8" t="s">
         <v>38</v>
       </c>
       <c r="N8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" ht="15" customHeight="1" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>59</v>
       </c>
@@ -3918,10 +4016,10 @@
         <v>39</v>
       </c>
       <c r="N9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="3:14" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" ht="15" customHeight="1" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>9</v>
       </c>
@@ -3944,10 +4042,10 @@
         <v>5</v>
       </c>
       <c r="N10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" ht="15" customHeight="1" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>60</v>
       </c>
@@ -3970,10 +4068,10 @@
         <v>69</v>
       </c>
       <c r="N11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" ht="15" customHeight="1" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>3</v>
       </c>
@@ -3993,7 +4091,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="13" ht="15" customHeight="1" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>62</v>
       </c>
@@ -4013,7 +4111,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="14" ht="15" customHeight="1" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>32</v>
       </c>
@@ -4033,7 +4131,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="15" ht="15" customHeight="1" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>17</v>
       </c>
@@ -4053,7 +4151,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="16" ht="15" customHeight="1" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>19</v>
       </c>
@@ -4073,7 +4171,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="17" ht="15" customHeight="1" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>35</v>
       </c>
@@ -4093,7 +4191,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="18" ht="15" customHeight="1" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>28</v>
       </c>
@@ -4113,7 +4211,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="19" ht="15" customHeight="1" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>61</v>
       </c>
@@ -4133,7 +4231,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="20" ht="15" customHeight="1" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>25</v>
       </c>
@@ -4153,7 +4251,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="21" ht="15" customHeight="1" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>21</v>
       </c>
@@ -4173,7 +4271,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="22" ht="15" customHeight="1" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>63</v>
       </c>
@@ -4193,7 +4291,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="23" ht="15" customHeight="1" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>44</v>
       </c>
@@ -4213,7 +4311,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="24" ht="15" customHeight="1" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>54</v>
       </c>
@@ -4233,7 +4331,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="25" ht="15" customHeight="1" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>64</v>
       </c>
@@ -4253,7 +4351,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="26" ht="15" customHeight="1" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>20</v>
       </c>
@@ -4273,7 +4371,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="27" ht="15" customHeight="1" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>22</v>
       </c>
@@ -4293,7 +4391,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="28" ht="15" customHeight="1" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>49</v>
       </c>
@@ -4307,13 +4405,13 @@
         <v>57</v>
       </c>
       <c r="L28" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="N28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="3:14" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" ht="15" customHeight="1" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>26</v>
       </c>
@@ -4324,13 +4422,13 @@
         <v>73</v>
       </c>
       <c r="L29" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="N29" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="4:14" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" ht="15" customHeight="1" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>37</v>
       </c>
@@ -4338,13 +4436,13 @@
         <v>11</v>
       </c>
       <c r="L30" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N30" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="4:14" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" ht="15" customHeight="1" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
         <v>73</v>
       </c>
@@ -4352,41 +4450,35 @@
         <v>31</v>
       </c>
       <c r="L31" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="N31" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="4:14" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" ht="15" customHeight="1" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
         <v>30</v>
       </c>
       <c r="I32" t="s">
         <v>22</v>
       </c>
-      <c r="L32" t="s">
-        <v>23</v>
-      </c>
       <c r="N32" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="4:14" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" ht="15" customHeight="1" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>43</v>
       </c>
       <c r="I33" t="s">
         <v>23</v>
       </c>
-      <c r="L33" t="s">
-        <v>52</v>
-      </c>
       <c r="N33" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="4:14" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" ht="15" customHeight="1" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>74</v>
       </c>
@@ -4394,10 +4486,10 @@
         <v>30</v>
       </c>
       <c r="N34" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="4:14" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" ht="15" customHeight="1" spans="4:14" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>52</v>
       </c>
@@ -4405,53 +4497,217 @@
         <v>8</v>
       </c>
       <c r="N35" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="9:14" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" ht="15" customHeight="1" spans="9:14" x14ac:dyDescent="0.25">
       <c r="I36" t="s">
         <v>72</v>
       </c>
       <c r="N36" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="9:14" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" ht="15" customHeight="1" spans="9:14" x14ac:dyDescent="0.25">
       <c r="I37" t="s">
         <v>14</v>
       </c>
       <c r="N37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="9:14" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" ht="15" customHeight="1" spans="9:14" x14ac:dyDescent="0.25">
       <c r="I38" t="s">
         <v>64</v>
       </c>
       <c r="N38" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="39" spans="9:9" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" ht="15" customHeight="1" spans="9:14" x14ac:dyDescent="0.25">
       <c r="I39" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="40" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="N39" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" ht="15" customHeight="1" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I40" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="41" ht="15" customHeight="1" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I41" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="42" ht="15" customHeight="1" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I42" t="s">
         <v>27</v>
       </c>
     </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:P13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="R3" sqref="R3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="11" max="11" width="64.42578125" customWidth="1"/>
+    <col min="12" max="12" width="79.42578125" customWidth="1"/>
+    <col min="14" max="14" width="71.140625" customWidth="1"/>
+    <col min="15" max="15" width="73.85546875" customWidth="1"/>
+    <col min="16" max="16" width="80.140625" customWidth="1"/>
+    <col min="17" max="17" width="46.85546875" customWidth="1"/>
+    <col min="18" max="18" width="60.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I3" t="s">
+        <v>88</v>
+      </c>
+      <c r="J3" t="s">
+        <v>94</v>
+      </c>
+      <c r="K3" t="s">
+        <v>89</v>
+      </c>
+      <c r="L3" t="s">
+        <v>90</v>
+      </c>
+      <c r="M3" t="s">
+        <v>137</v>
+      </c>
+      <c r="N3" t="s">
+        <v>133</v>
+      </c>
+      <c r="O3" t="s">
+        <v>139</v>
+      </c>
+      <c r="P3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>142</v>
+      </c>
+      <c r="L4" t="s">
+        <v>143</v>
+      </c>
+      <c r="M4" t="s">
+        <v>144</v>
+      </c>
+      <c r="N4" t="s">
+        <v>145</v>
+      </c>
+      <c r="O4" t="s">
+        <v>146</v>
+      </c>
+      <c r="P4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>148</v>
+      </c>
+      <c r="N5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>150</v>
+      </c>
+      <c r="N6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L7" t="s">
+        <v>152</v>
+      </c>
+      <c r="N7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>154</v>
+      </c>
+      <c r="N8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>156</v>
+      </c>
+      <c r="N9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>158</v>
+      </c>
+      <c r="N10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="11" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="N11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N12" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="14:14" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added functionality to detect canceled games
</commit_message>
<xml_diff>
--- a/data/AHLdelegacije.xlsx
+++ b/data/AHLdelegacije.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet sheetId="1" name="AHL" state="visible" r:id="rId4"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="139">
   <si>
     <t>BULOVEC</t>
   </si>
@@ -147,76 +147,79 @@
     <t>SLAVIERO</t>
   </si>
   <si>
+    <t>HEAD</t>
+  </si>
+  <si>
+    <t>SPIEGEL</t>
+  </si>
+  <si>
+    <t>BRUNNER</t>
+  </si>
+  <si>
+    <t>LOICHT</t>
+  </si>
+  <si>
+    <t>MATTHEY</t>
+  </si>
+  <si>
+    <t>VOICAN</t>
+  </si>
+  <si>
+    <t>BAJT</t>
+  </si>
+  <si>
+    <t>LESNIAK</t>
+  </si>
+  <si>
+    <t>BERGANT</t>
+  </si>
+  <si>
+    <t>JAVORNIK</t>
+  </si>
+  <si>
+    <t>EGGER</t>
+  </si>
+  <si>
+    <t>FLEISCHMANN</t>
+  </si>
+  <si>
+    <t>PAHOR</t>
+  </si>
+  <si>
+    <t>ARLIC</t>
+  </si>
+  <si>
+    <t>OREL</t>
+  </si>
+  <si>
+    <t>PÖTSCHER</t>
+  </si>
+  <si>
+    <t>SCHWEIGHOFER</t>
+  </si>
+  <si>
+    <t>EISL</t>
+  </si>
+  <si>
+    <t>MOIDL</t>
+  </si>
+  <si>
+    <t>REISINGER</t>
+  </si>
+  <si>
+    <t>WUNTSCHEK</t>
+  </si>
+  <si>
+    <t>PUFF</t>
+  </si>
+  <si>
+    <t>HLAVATY</t>
+  </si>
+  <si>
     <t>LINESMAN</t>
   </si>
   <si>
-    <t>HEAD</t>
-  </si>
-  <si>
-    <t>SPIEGEL</t>
-  </si>
-  <si>
-    <t>BRUNNER</t>
-  </si>
-  <si>
-    <t>LOICHT</t>
-  </si>
-  <si>
-    <t>MATTHEY</t>
-  </si>
-  <si>
-    <t>VOICAN</t>
-  </si>
-  <si>
-    <t>BAJT</t>
-  </si>
-  <si>
-    <t>LESNIAK</t>
-  </si>
-  <si>
-    <t>BERGANT</t>
-  </si>
-  <si>
-    <t>JAVORNIK</t>
-  </si>
-  <si>
-    <t>EGGER</t>
-  </si>
-  <si>
-    <t>FLEISCHMANN</t>
-  </si>
-  <si>
-    <t>PAHOR</t>
-  </si>
-  <si>
-    <t>ARLIC</t>
-  </si>
-  <si>
-    <t>OREL</t>
-  </si>
-  <si>
-    <t>PÖTSCHER</t>
-  </si>
-  <si>
-    <t>SCHWEIGHOFER</t>
-  </si>
-  <si>
-    <t>EISL</t>
-  </si>
-  <si>
-    <t>MOIDL</t>
-  </si>
-  <si>
-    <t>REISINGER</t>
-  </si>
-  <si>
-    <t>WUNTSCHEK</t>
-  </si>
-  <si>
-    <t>PUFF</t>
-  </si>
-  <si>
-    <t>HLAVATY</t>
+    <t>HEINRICHER</t>
   </si>
   <si>
     <t>2020-10-03</t>
@@ -231,24 +234,36 @@
     <t>2020-10-10</t>
   </si>
   <si>
+    <t>2020-10-17</t>
+  </si>
+  <si>
+    <t>2020-10-14</t>
+  </si>
+  <si>
+    <t>2020-10-22</t>
+  </si>
+  <si>
+    <t>2020-10-24</t>
+  </si>
+  <si>
+    <t>2020-10-31</t>
+  </si>
+  <si>
+    <t>2020-10-30</t>
+  </si>
+  <si>
+    <t>2020-11-01</t>
+  </si>
+  <si>
     <t>zbrisano</t>
   </si>
   <si>
-    <t>2020-10-14</t>
-  </si>
-  <si>
-    <t>2020-10-17</t>
-  </si>
-  <si>
-    <t>2020-10-22</t>
-  </si>
-  <si>
-    <t>2020-10-24</t>
-  </si>
-  <si>
     <t>2020-10-21</t>
   </si>
   <si>
+    <t>2020-10-29</t>
+  </si>
+  <si>
     <t>Hala Tivoli;BULOVEC;REZEK;MIKLIC;SNOJ</t>
   </si>
   <si>
@@ -270,10 +285,22 @@
     <t>Eishalle Dornbirn;HOLZER;SCHAUER;EISL;HUBER</t>
   </si>
   <si>
-    <t>Eishalle Jesenice;LESNIAK;REZEK;JAVORNIK;SNOJ</t>
-  </si>
-  <si>
-    <t>Hala Tivoli;BAJT;REZEK;ARLIC;JAVORNIK</t>
+    <t>Linz AG Eisarena;BRUNNER;LEHNER;MOIDL;REISINGER</t>
+  </si>
+  <si>
+    <t>Hala Tivoli;BAJT;REZEK;JAVORNIK;SNOJ</t>
+  </si>
+  <si>
+    <t>Eishalle Gröden;MOSCHEN;PINIE;DE ZORDO;FLEISCHMANN</t>
+  </si>
+  <si>
+    <t>Eisarena Salzburg;BRUNNER;KUMMER;MATTHEY;REISINGER</t>
+  </si>
+  <si>
+    <t>Eishalle Ritten;BENVEGNU;LEGA;BEDANA;LINESMAN</t>
+  </si>
+  <si>
+    <t>Klagenfurter Stadthalle;OREL;PODLESNIK;PÖTSCHER;SCHWEIGHOFER</t>
   </si>
   <si>
     <t>Eishalle Gröden;LAZZERI;PINIE;BASSO;PIRAS</t>
@@ -291,12 +318,18 @@
     <t>Eishalle Gröden;BENVEGNU;LEGA;BASSO;DE ZORDO</t>
   </si>
   <si>
-    <t>Linz AG Eisarena;BRUNNER;LEHNER;MOIDL;REISINGER</t>
+    <t>Sportpark Kitzbühel;HUBER;RUETZ;MARTIN;SPIEGEL</t>
   </si>
   <si>
     <t>Klagenfurter Stadthalle;PODLESNIK;WUNTSCHEK;HOLZER;PUFF</t>
   </si>
   <si>
+    <t>Eishalle Jesenice;PAHOR;REZEK;PAGON;SNOJ</t>
+  </si>
+  <si>
+    <t>Eishalle Jesenice;FAJDIGA;LESNIAK;ARLIC;JAVORNIK</t>
+  </si>
+  <si>
     <t>Linz AG Eisarena;DURCHNER;FICHTNER;KAINBERGER;WIMMLER</t>
   </si>
   <si>
@@ -312,12 +345,15 @@
     <t>Klagenfurter Stadthalle;DURCHNER;OREL;LEGAT;PÖTSCHER</t>
   </si>
   <si>
-    <t>Sportpark Kitzbühel;HUBER;RUETZ;MARTIN;SPIEGEL</t>
+    <t>Eishalle Ritten;GIACOMOZZI;MOSCHEN;CRISTELI;DE ZORDO</t>
   </si>
   <si>
     <t>Eisarena Salzburg;FICHTNER;HLAVATY;KAINBERGER;LEGAT</t>
   </si>
   <si>
+    <t>Sportpark Kitzbühel;HEINRICHER;WIDMANN;EISL;HUBER</t>
+  </si>
+  <si>
     <t>Eishalle Sterzing;GIACOMOZZI;VIRTA;MANTOVANI;RIGONI</t>
   </si>
   <si>
@@ -333,10 +369,13 @@
     <t>Eisarena Salzburg;WALLNER;WIDMANN;KAINBERGER;SCHWEIGHOFER</t>
   </si>
   <si>
-    <t>Eishalle Ritten;GIACOMOZZI;MOSCHEN;CRISTELI;DE ZORDO</t>
-  </si>
-  <si>
-    <t>Eishalle Sterzing;BENVEGNU;EGGER;CRISTELI;FLEISCHMANN</t>
+    <t>Eishalle Bruneck;LEGA;STEFENELLI;BASSO;PIRAS</t>
+  </si>
+  <si>
+    <t>Eishalle Ritten;MOSCHEN;STEFENELLI;DE ZORDO;PIRAS</t>
+  </si>
+  <si>
+    <t>Eishalle Sterzing;EGGER;STEFENELLI;CRISTELI;DE ZORDO</t>
   </si>
   <si>
     <t>Eishalle Dornbirn;HUBER;SCHAUER;HUBER;MARTIN</t>
@@ -354,10 +393,10 @@
     <t>Eishalle Sterzing;LAZZERI;STEFENELLI;RIGONI;SLAVIERO</t>
   </si>
   <si>
-    <t>Eishalle Bruneck;LEGA;STEFENELLI;BASSO;PIRAS</t>
-  </si>
-  <si>
-    <t>Eishalle Lustenau;HOLZER;SCHAUER;RINKER;SPIEGEL</t>
+    <t>Eishalle Asiago;GIACOMOZZI;LAZZERI;CRISTELI;FLEISCHMANN</t>
+  </si>
+  <si>
+    <t>Eishalle Bruneck;GIACOMOZZI;LAZZERI;FLEISCHMANN;PIRAS</t>
   </si>
   <si>
     <t>Eishalle Feldkirch;BERNEKER;RUETZ;RINKER;TSCHREPITSCH</t>
@@ -375,12 +414,6 @@
     <t>Eishalle Feldkirch;HUBER;RUETZ;EISL;SPIEGEL</t>
   </si>
   <si>
-    <t>Eishalle Cortina;LAZZERI;PINIE;DE ZORDO;FLEISCHMANN</t>
-  </si>
-  <si>
-    <t>Eishalle Ritten;MOSCHEN;STEFENELLI;DE ZORDO;PIRAS</t>
-  </si>
-  <si>
     <t>Eishalle Bruneck;LEGA;MOSCHEN;BEDANA;DE ZORDO</t>
   </si>
   <si>
@@ -391,9 +424,6 @@
   </si>
   <si>
     <t>Eishalle Lustenau;HOLZER;SCHAUER;MARTIN;RINKER</t>
-  </si>
-  <si>
-    <t>Eishalle Asiago;GIACOMOZZI;LAZZERI;CRISTELI;FLEISCHMANN</t>
   </si>
   <si>
     <t>Eishalle Asiago;LAZZERI;PINIE;BASSO;RIGONI</t>
@@ -720,10 +750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:BP56"/>
+  <dimension ref="A3:BQ56"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="BA5" sqref="BA5"/>
+      <selection activeCell="AO6" sqref="AO6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" customHeight="1"/>
@@ -771,34 +801,33 @@
     <col min="41" max="41" width="12" customWidth="1"/>
     <col min="42" max="42" width="11.42578125" customWidth="1"/>
     <col min="43" max="43" width="14.42578125" customWidth="1"/>
-    <col min="44" max="44" width="12" customWidth="1"/>
-    <col min="45" max="45" width="10.140625" customWidth="1"/>
-    <col min="46" max="46" width="10.5703125" customWidth="1"/>
-    <col min="47" max="47" width="13" customWidth="1"/>
-    <col min="48" max="48" width="11.7109375" customWidth="1"/>
-    <col min="49" max="49" width="14.28515625" customWidth="1"/>
-    <col min="50" max="50" width="16.85546875" customWidth="1"/>
-    <col min="51" max="51" width="12.7109375" customWidth="1"/>
-    <col min="52" max="52" width="13.42578125" customWidth="1"/>
-    <col min="53" max="54" width="10.28515625" customWidth="1"/>
-    <col min="55" max="55" width="12.140625" customWidth="1"/>
-    <col min="56" max="56" width="12" customWidth="1"/>
-    <col min="57" max="57" width="9.28515625" customWidth="1"/>
-    <col min="58" max="58" width="11.7109375" customWidth="1"/>
-    <col min="59" max="59" width="10.28515625" customWidth="1"/>
-    <col min="60" max="60" width="15.140625" customWidth="1"/>
-    <col min="61" max="61" width="11.28515625" customWidth="1"/>
-    <col min="62" max="62" width="10.5703125" customWidth="1"/>
-    <col min="63" max="63" width="11" customWidth="1"/>
-    <col min="64" max="64" width="11.7109375" customWidth="1"/>
-    <col min="66" max="66" width="12.5703125" customWidth="1"/>
-    <col min="67" max="67" width="14.140625" customWidth="1"/>
-    <col min="69" max="69" width="13.7109375" customWidth="1"/>
-    <col min="71" max="71" width="20.140625" customWidth="1"/>
-    <col min="73" max="73" width="10.140625" customWidth="1"/>
+    <col min="44" max="44" width="10.140625" customWidth="1"/>
+    <col min="45" max="45" width="10.5703125" customWidth="1"/>
+    <col min="46" max="46" width="13" customWidth="1"/>
+    <col min="47" max="47" width="11.7109375" customWidth="1"/>
+    <col min="48" max="48" width="14.28515625" customWidth="1"/>
+    <col min="49" max="49" width="16.85546875" customWidth="1"/>
+    <col min="50" max="50" width="12.7109375" customWidth="1"/>
+    <col min="51" max="51" width="13.42578125" customWidth="1"/>
+    <col min="52" max="53" width="10.28515625" customWidth="1"/>
+    <col min="54" max="54" width="12.140625" customWidth="1"/>
+    <col min="55" max="55" width="23.28515625" customWidth="1"/>
+    <col min="56" max="56" width="9.28515625" customWidth="1"/>
+    <col min="57" max="57" width="11.7109375" customWidth="1"/>
+    <col min="58" max="58" width="10.28515625" customWidth="1"/>
+    <col min="59" max="59" width="15.140625" customWidth="1"/>
+    <col min="60" max="60" width="11.28515625" customWidth="1"/>
+    <col min="61" max="61" width="10.5703125" customWidth="1"/>
+    <col min="62" max="62" width="11" customWidth="1"/>
+    <col min="63" max="63" width="11.7109375" customWidth="1"/>
+    <col min="65" max="65" width="12.5703125" customWidth="1"/>
+    <col min="66" max="66" width="14.140625" customWidth="1"/>
+    <col min="68" max="68" width="13.7109375" customWidth="1"/>
+    <col min="70" max="70" width="20.140625" customWidth="1"/>
+    <col min="72" max="72" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="15" customHeight="1" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="3" ht="15" customHeight="1" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1000,199 +1029,202 @@
       <c r="BO3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="4" ht="15" customHeight="1" spans="1:67" x14ac:dyDescent="0.25">
+      <c r="BP3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="P4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Q4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="R4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="S4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="T4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="U4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="V4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="W4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="X4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Y4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Z4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AA4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AB4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AC4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AD4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AE4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AT4" t="s">
         <v>69</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AU4" t="s">
         <v>69</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AV4" t="s">
         <v>69</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AW4" t="s">
         <v>69</v>
       </c>
-      <c r="AI4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>71</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>71</v>
-      </c>
-      <c r="AS4" t="s">
-        <v>71</v>
-      </c>
-      <c r="AT4" t="s">
+      <c r="AX4" t="s">
+        <v>69</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>69</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>69</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>69</v>
+      </c>
+      <c r="BB4" t="s">
+        <v>69</v>
+      </c>
+      <c r="BC4" t="s">
+        <v>69</v>
+      </c>
+      <c r="BD4" t="s">
         <v>72</v>
       </c>
-      <c r="AU4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AV4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AW4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AX4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AY4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AZ4" t="s">
-        <v>68</v>
-      </c>
-      <c r="BA4" t="s">
-        <v>68</v>
-      </c>
-      <c r="BB4" t="s">
-        <v>68</v>
-      </c>
-      <c r="BC4" t="s">
-        <v>68</v>
-      </c>
-      <c r="BD4" t="s">
-        <v>68</v>
-      </c>
       <c r="BE4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="BF4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="BG4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="BH4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="BI4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="BJ4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="BK4" t="s">
         <v>74</v>
       </c>
       <c r="BL4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="BM4" t="s">
         <v>75</v>
@@ -1201,170 +1233,188 @@
         <v>75</v>
       </c>
       <c r="BO4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" ht="15" customHeight="1" spans="1:67" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="BP4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" t="s">
         <v>69</v>
       </c>
-      <c r="B5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G5" t="s">
-        <v>68</v>
-      </c>
       <c r="H5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="N5" t="s">
         <v>74</v>
       </c>
       <c r="O5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="P5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Q5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="R5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="S5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="T5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="U5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="V5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="W5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="X5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Y5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="Z5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AA5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AB5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AC5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AD5" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>77</v>
       </c>
       <c r="AF5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AH5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AI5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AJ5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AK5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AL5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AO5" t="s">
         <v>74</v>
       </c>
       <c r="AP5" t="s">
-        <v>73</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AR5" t="s">
         <v>71</v>
       </c>
       <c r="AS5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AT5" t="s">
-        <v>73</v>
-      </c>
-      <c r="AU5" t="s">
         <v>74</v>
       </c>
+      <c r="AV5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>75</v>
+      </c>
       <c r="AY5" t="s">
+        <v>78</v>
+      </c>
+      <c r="BA5" t="s">
         <v>75</v>
       </c>
-      <c r="AZ5" t="s">
-        <v>74</v>
-      </c>
       <c r="BB5" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="BC5" t="s">
         <v>75</v>
       </c>
       <c r="BD5" t="s">
-        <v>74</v>
+        <v>76</v>
+      </c>
+      <c r="BE5" t="s">
+        <v>79</v>
       </c>
       <c r="BF5" t="s">
-        <v>75</v>
-      </c>
-      <c r="BJ5" t="s">
+        <v>78</v>
+      </c>
+      <c r="BG5" t="s">
+        <v>78</v>
+      </c>
+      <c r="BH5" t="s">
+        <v>78</v>
+      </c>
+      <c r="BI5" t="s">
+        <v>80</v>
+      </c>
+      <c r="BK5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="6" ht="15" customHeight="1" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" t="s">
-        <v>75</v>
       </c>
       <c r="F6" t="s">
         <v>74</v>
@@ -1373,99 +1423,111 @@
         <v>74</v>
       </c>
       <c r="H6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="L6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="N6" t="s">
         <v>75</v>
       </c>
       <c r="O6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="P6" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q6" t="s">
         <v>69</v>
       </c>
-      <c r="Q6" t="s">
-        <v>68</v>
-      </c>
       <c r="R6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="T6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="U6" t="s">
+        <v>73</v>
+      </c>
+      <c r="W6" t="s">
         <v>72</v>
       </c>
-      <c r="W6" t="s">
-        <v>73</v>
-      </c>
       <c r="X6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Y6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Z6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AA6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AB6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AC6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AD6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AF6" t="s">
         <v>75</v>
       </c>
       <c r="AH6" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>76</v>
       </c>
       <c r="AL6" t="s">
         <v>75</v>
       </c>
-      <c r="AQ6" t="s">
-        <v>71</v>
-      </c>
-      <c r="AR6" t="s">
-        <v>71</v>
-      </c>
       <c r="AS6" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="AT6" t="s">
-        <v>74</v>
+        <v>77</v>
+      </c>
+      <c r="BA6" t="s">
+        <v>78</v>
       </c>
       <c r="BB6" t="s">
-        <v>74</v>
-      </c>
-      <c r="BD6" t="s">
+        <v>76</v>
+      </c>
+      <c r="BC6" t="s">
+        <v>81</v>
+      </c>
+      <c r="BE6" t="s">
+        <v>78</v>
+      </c>
+      <c r="BI6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="7" ht="15" customHeight="1" spans="2:56" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>74</v>
-      </c>
       <c r="D7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F7" t="s">
         <v>75</v>
@@ -1474,81 +1536,84 @@
         <v>75</v>
       </c>
       <c r="H7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I7" t="s">
         <v>75</v>
       </c>
       <c r="J7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="O7" t="s">
+        <v>70</v>
+      </c>
+      <c r="P7" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>72</v>
+      </c>
+      <c r="R7" t="s">
         <v>69</v>
       </c>
-      <c r="P7" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>73</v>
-      </c>
-      <c r="R7" t="s">
-        <v>68</v>
-      </c>
       <c r="T7" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="U7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W7" t="s">
         <v>74</v>
       </c>
       <c r="X7" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y7" t="s">
         <v>69</v>
       </c>
-      <c r="Y7" t="s">
-        <v>68</v>
-      </c>
       <c r="Z7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AA7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AB7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AC7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AD7" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>78</v>
       </c>
       <c r="AH7" t="s">
-        <v>72</v>
-      </c>
-      <c r="AR7" t="s">
-        <v>71</v>
-      </c>
-      <c r="AS7" t="s">
-        <v>70</v>
-      </c>
-      <c r="AT7" t="s">
+        <v>73</v>
+      </c>
+      <c r="BC7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" t="s">
         <v>75</v>
       </c>
-      <c r="BD7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" ht="15" customHeight="1" spans="2:56" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>75</v>
+      <c r="F8" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" t="s">
+        <v>76</v>
       </c>
       <c r="J8" t="s">
         <v>75</v>
@@ -1557,64 +1622,58 @@
         <v>74</v>
       </c>
       <c r="O8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Q8" t="s">
+        <v>80</v>
+      </c>
+      <c r="R8" t="s">
+        <v>72</v>
+      </c>
+      <c r="T8" t="s">
+        <v>74</v>
+      </c>
+      <c r="W8" t="s">
         <v>76</v>
       </c>
-      <c r="R8" t="s">
-        <v>73</v>
-      </c>
-      <c r="T8" t="s">
-        <v>73</v>
-      </c>
-      <c r="U8" t="s">
-        <v>75</v>
-      </c>
       <c r="X8" t="s">
-        <v>68</v>
+        <v>69</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>76</v>
       </c>
       <c r="Z8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AA8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AB8" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="AC8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AD8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AH8" t="s">
-        <v>73</v>
-      </c>
-      <c r="AR8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" ht="15" customHeight="1" spans="2:44" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" ht="15" customHeight="1" spans="2:34" x14ac:dyDescent="0.25">
       <c r="L9" t="s">
         <v>75</v>
       </c>
       <c r="P9" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="R9" t="s">
         <v>74</v>
       </c>
-      <c r="T9" t="s">
-        <v>74</v>
-      </c>
       <c r="X9" t="s">
         <v>74</v>
       </c>
@@ -1622,24 +1681,21 @@
         <v>74</v>
       </c>
       <c r="AA9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AC9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" ht="15" customHeight="1" spans="12:34" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>76</v>
+      </c>
+      <c r="P10" t="s">
         <v>73</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>71</v>
-      </c>
-      <c r="AH9" t="s">
-        <v>76</v>
-      </c>
-      <c r="AR9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" ht="15" customHeight="1" spans="12:44" x14ac:dyDescent="0.25">
-      <c r="P10" t="s">
-        <v>72</v>
       </c>
       <c r="X10" t="s">
         <v>75</v>
@@ -1648,7 +1704,7 @@
         <v>75</v>
       </c>
       <c r="AA10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AC10" t="s">
         <v>74</v>
@@ -1657,25 +1713,28 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" ht="15" customHeight="1" spans="16:34" x14ac:dyDescent="0.25">
+    <row r="11" ht="15" customHeight="1" spans="12:34" x14ac:dyDescent="0.25">
       <c r="P11" t="s">
-        <v>68</v>
+        <v>69</v>
+      </c>
+      <c r="X11" t="s">
+        <v>81</v>
       </c>
       <c r="Z11" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" ht="15" customHeight="1" spans="16:34" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" ht="15" customHeight="1" spans="16:26" x14ac:dyDescent="0.25">
       <c r="P12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" ht="15" customHeight="1" spans="16:16" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" ht="15" customHeight="1" spans="16:26" x14ac:dyDescent="0.25">
       <c r="P13" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" ht="15" customHeight="1" spans="16:16" x14ac:dyDescent="0.25">
@@ -1683,8 +1742,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" ht="15" customHeight="1" spans="16:16" x14ac:dyDescent="0.25"/>
-    <row r="16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" ht="15" customHeight="1" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" ht="15" customHeight="1" spans="16:16" x14ac:dyDescent="0.25"/>
     <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1731,10 +1794,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:I42"/>
+  <dimension ref="A3:M42"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" customHeight="1"/>
@@ -1755,27 +1818,27 @@
     <col min="16" max="16" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" ht="15" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" t="s">
         <v>69</v>
       </c>
-      <c r="C3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>72</v>
       </c>
-      <c r="E3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" t="s">
-        <v>73</v>
-      </c>
       <c r="G3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="H3" t="s">
         <v>74</v>
@@ -1783,8 +1846,20 @@
       <c r="I3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="4" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>81</v>
+      </c>
+      <c r="K3" t="s">
+        <v>77</v>
+      </c>
+      <c r="L3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1798,7 +1873,7 @@
         <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
         <v>34</v>
@@ -1807,13 +1882,25 @@
         <v>33</v>
       </c>
       <c r="H4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="J4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L4" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1827,22 +1914,34 @@
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G5" t="s">
         <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="I5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1856,22 +1955,34 @@
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" t="s">
         <v>61</v>
       </c>
-      <c r="H6" t="s">
-        <v>53</v>
-      </c>
       <c r="I6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="J6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1882,10 +1993,10 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F7" t="s">
         <v>35</v>
@@ -1894,13 +2005,25 @@
         <v>15</v>
       </c>
       <c r="H7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" t="s">
         <v>3</v>
       </c>
-      <c r="I7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7" t="s">
+        <v>62</v>
+      </c>
+      <c r="L7" t="s">
+        <v>66</v>
+      </c>
+      <c r="M7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1911,19 +2034,25 @@
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F8" t="s">
         <v>4</v>
       </c>
       <c r="H8" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="I8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>55</v>
+      </c>
+      <c r="M8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" ht="15" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1934,19 +2063,25 @@
         <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F9" t="s">
         <v>22</v>
       </c>
       <c r="H9" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="I9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1</v>
+      </c>
+      <c r="M9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" ht="15" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1957,19 +2092,25 @@
         <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F10" t="s">
         <v>28</v>
       </c>
       <c r="H10" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="I10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>35</v>
+      </c>
+      <c r="M10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" ht="15" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1980,19 +2121,25 @@
         <v>37</v>
       </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F11" t="s">
         <v>25</v>
       </c>
       <c r="H11" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="I11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="L11" t="s">
+        <v>3</v>
+      </c>
+      <c r="M11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" ht="15" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -2009,13 +2156,16 @@
         <v>7</v>
       </c>
       <c r="H12" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" ht="15" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -2029,16 +2179,19 @@
         <v>16</v>
       </c>
       <c r="F13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H13" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="I13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="L13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" ht="15" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -2055,13 +2208,16 @@
         <v>37</v>
       </c>
       <c r="H14" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" ht="15" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -2075,16 +2231,19 @@
         <v>17</v>
       </c>
       <c r="F15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H15" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="I15" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" ht="15" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -2095,19 +2254,22 @@
         <v>40</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F16" t="s">
         <v>41</v>
       </c>
       <c r="H16" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="I16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="L16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" ht="15" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -2124,13 +2286,16 @@
         <v>36</v>
       </c>
       <c r="H17" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="I17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="L17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" ht="15" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -2147,13 +2312,16 @@
         <v>9</v>
       </c>
       <c r="H18" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" t="s">
+        <v>25</v>
+      </c>
+      <c r="L18" t="s">
         <v>13</v>
       </c>
-      <c r="I18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" ht="15" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -2167,16 +2335,19 @@
         <v>25</v>
       </c>
       <c r="F19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" t="s">
+        <v>6</v>
+      </c>
+      <c r="L19" t="s">
         <v>25</v>
       </c>
-      <c r="I19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" ht="15" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -2192,14 +2363,14 @@
       <c r="F20" t="s">
         <v>26</v>
       </c>
-      <c r="H20" t="s">
-        <v>22</v>
-      </c>
       <c r="I20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="L20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" ht="15" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -2215,14 +2386,14 @@
       <c r="F21" t="s">
         <v>5</v>
       </c>
-      <c r="H21" t="s">
-        <v>5</v>
-      </c>
       <c r="I21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="L21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" ht="15" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -2233,19 +2404,19 @@
         <v>15</v>
       </c>
       <c r="E22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F22" t="s">
         <v>29</v>
       </c>
-      <c r="H22" t="s">
-        <v>28</v>
-      </c>
       <c r="I22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="L22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" ht="15" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -2261,14 +2432,14 @@
       <c r="F23" t="s">
         <v>42</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
+        <v>54</v>
+      </c>
+      <c r="L23" t="s">
         <v>6</v>
       </c>
-      <c r="I23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" ht="15" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -2284,14 +2455,8 @@
       <c r="F24" t="s">
         <v>15</v>
       </c>
-      <c r="H24" t="s">
-        <v>26</v>
-      </c>
-      <c r="I24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" ht="15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -2307,14 +2472,8 @@
       <c r="F25" t="s">
         <v>19</v>
       </c>
-      <c r="H25" t="s">
-        <v>27</v>
-      </c>
-      <c r="I25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" ht="15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -2328,16 +2487,10 @@
         <v>13</v>
       </c>
       <c r="F26" t="s">
-        <v>61</v>
-      </c>
-      <c r="H26" t="s">
-        <v>25</v>
-      </c>
-      <c r="I26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" ht="15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -2351,16 +2504,10 @@
         <v>14</v>
       </c>
       <c r="F27" t="s">
-        <v>45</v>
-      </c>
-      <c r="H27" t="s">
-        <v>55</v>
-      </c>
-      <c r="I27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" ht="15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -2373,11 +2520,8 @@
       <c r="F28" t="s">
         <v>33</v>
       </c>
-      <c r="I28" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" ht="15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -2390,11 +2534,8 @@
       <c r="F29" t="s">
         <v>16</v>
       </c>
-      <c r="I29" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" ht="15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -2407,11 +2548,8 @@
       <c r="F30" t="s">
         <v>17</v>
       </c>
-      <c r="I30" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" ht="15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>25</v>
       </c>
@@ -2424,11 +2562,8 @@
       <c r="F31" t="s">
         <v>20</v>
       </c>
-      <c r="I31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -2436,7 +2571,7 @@
         <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2447,7 +2582,7 @@
         <v>23</v>
       </c>
       <c r="C33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2486,10 +2621,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:I13"/>
+  <dimension ref="A3:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="96" zoomScaleNormal="130">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" customHeight="1"/>
@@ -2500,6 +2635,8 @@
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="12.140625" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="41" customWidth="1"/>
+    <col min="8" max="8" width="58.28515625" customWidth="1"/>
     <col min="9" max="9" width="62.5703125" customWidth="1"/>
     <col min="10" max="10" width="79.42578125" customWidth="1"/>
     <col min="11" max="11" width="74" customWidth="1"/>
@@ -2552,27 +2689,27 @@
     <col min="64" max="64" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" ht="15" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" t="s">
         <v>69</v>
       </c>
-      <c r="C3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>72</v>
       </c>
-      <c r="E3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" t="s">
-        <v>73</v>
-      </c>
       <c r="G3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="H3" t="s">
         <v>74</v>
@@ -2580,177 +2717,204 @@
       <c r="I3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="4" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>81</v>
+      </c>
+      <c r="K3" t="s">
+        <v>77</v>
+      </c>
+      <c r="L3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="E4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="G4" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="H4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="I4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="J4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K4" t="s">
+        <v>92</v>
+      </c>
+      <c r="L4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E5" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="F5" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="H5" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="L5" t="s">
+        <v>102</v>
+      </c>
+      <c r="M5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="E6" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="F6" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="H6" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="I6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="L6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="E7" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="F7" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="H7" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="I7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="L7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="C8" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="E8" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="F8" t="s">
-        <v>111</v>
-      </c>
-      <c r="H8" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="I8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="L8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" ht="15" customHeight="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="C9" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="E9" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="F9" t="s">
-        <v>118</v>
-      </c>
-      <c r="H9" t="s">
-        <v>119</v>
-      </c>
-      <c r="I9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" ht="15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="B10" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="C10" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="F10" t="s">
-        <v>124</v>
-      </c>
-      <c r="I10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="11" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="B11" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="C11" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
6-11 added new counter
</commit_message>
<xml_diff>
--- a/data/AHLdelegacije.xlsx
+++ b/data/AHLdelegacije.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="158">
   <si>
     <t>BULOVEC</t>
   </si>
@@ -216,6 +216,15 @@
     <t>HLAVATY</t>
   </si>
   <si>
+    <t>VIGNOLO</t>
+  </si>
+  <si>
+    <t>HEINRICHER</t>
+  </si>
+  <si>
+    <t>Ricco</t>
+  </si>
+  <si>
     <t>2020-10-03</t>
   </si>
   <si>
@@ -240,6 +249,9 @@
     <t>2020-10-24</t>
   </si>
   <si>
+    <t>2020-11-14</t>
+  </si>
+  <si>
     <t>2020-10-30</t>
   </si>
   <si>
@@ -249,6 +261,9 @@
     <t>2020-11-08</t>
   </si>
   <si>
+    <t>2020-11-12</t>
+  </si>
+  <si>
     <t>zbrisano</t>
   </si>
   <si>
@@ -264,6 +279,9 @@
     <t>2020-10-29</t>
   </si>
   <si>
+    <t>2020-11-15</t>
+  </si>
+  <si>
     <t>Hala Tivoli;BULOVEC;REZEK;MIKLIC;SNOJ</t>
   </si>
   <si>
@@ -309,6 +327,15 @@
     <t>Linz AG Eisarena;BRUNNER;LOICHT;MOIDL;VOICAN</t>
   </si>
   <si>
+    <t>Hala Tivoli;LESNIAK;PAHOR;PAGON;SNOJ</t>
+  </si>
+  <si>
+    <t>Hala Tivoli;FAJDIGA;REZEK;ARLIC;BERGANT</t>
+  </si>
+  <si>
+    <t>Eishalle Feldkirch;HOLZER;HUBER;HUBER;SPIEGEL</t>
+  </si>
+  <si>
     <t>Eishalle Gröden;LAZZERI;PINIE;BASSO;PIRAS</t>
   </si>
   <si>
@@ -339,6 +366,12 @@
     <t>Eishalle Asiago;EGGER;GIACOMOZZI;FLEISCHMANN;PIRAS</t>
   </si>
   <si>
+    <t>Eishalle Sterzing;BENVEGNU;EGGER;CRISTELI;DE ZORDO</t>
+  </si>
+  <si>
+    <t>Eishalle Canazei;GIACOMOZZI;LEGA;CRISTELI;VIGNOLO</t>
+  </si>
+  <si>
     <t>Linz AG Eisarena;DURCHNER;FICHTNER;KAINBERGER;WIMMLER</t>
   </si>
   <si>
@@ -360,6 +393,12 @@
     <t>Eisarena Salzburg;FICHTNER;HLAVATY;KAINBERGER;LEGAT</t>
   </si>
   <si>
+    <t>Eishalle Asiago;GIACOMOZZI;MOSCHEN;FLEISCHMANN;PIRAS</t>
+  </si>
+  <si>
+    <t>Eishalle Lustenau;HUBER;WALLNER;EISL;KAINBERGER</t>
+  </si>
+  <si>
     <t>Eishalle Sterzing;GIACOMOZZI;VIRTA;MANTOVANI;RIGONI</t>
   </si>
   <si>
@@ -381,6 +420,12 @@
     <t>Eishalle Ritten;MOSCHEN;STEFENELLI;DE ZORDO;PIRAS</t>
   </si>
   <si>
+    <t>Eishalle Cortina;LEGA;STEFENELLI;BEDANA;MANTOVANI</t>
+  </si>
+  <si>
+    <t>Sportpark Kitzbühel;DURCHNER;HLAVATY;LEGAT;WEISS</t>
+  </si>
+  <si>
     <t>Eishalle Dornbirn;HUBER;SCHAUER;HUBER;MARTIN</t>
   </si>
   <si>
@@ -399,6 +444,9 @@
     <t>Eishalle Asiago;GIACOMOZZI;LAZZERI;CRISTELI;FLEISCHMANN</t>
   </si>
   <si>
+    <t>Eishalle Feldkirch;HEINRICHER;PODLESNIK;PÖTSCHER;SCHWEIGHOFER</t>
+  </si>
+  <si>
     <t>Eishalle Feldkirch;BERNEKER;RUETZ;RINKER;TSCHREPITSCH</t>
   </si>
   <si>
@@ -414,6 +462,9 @@
     <t>Eishalle Feldkirch;HUBER;RUETZ;EISL;SPIEGEL</t>
   </si>
   <si>
+    <t>Eishalle Dornbirn;HOLZER;SCHAUER;RINKER;SPIEGEL</t>
+  </si>
+  <si>
     <t>Eishalle Bruneck;LEGA;MOSCHEN;BEDANA;DE ZORDO</t>
   </si>
   <si>
@@ -426,6 +477,9 @@
     <t>Eishalle Lustenau;HOLZER;SCHAUER;MARTIN;RINKER</t>
   </si>
   <si>
+    <t>Eishalle Asiago;BENVEGNU;EGGER;BEDANA;FLEISCHMANN</t>
+  </si>
+  <si>
     <t>Eishalle Asiago;LAZZERI;PINIE;BASSO;RIGONI</t>
   </si>
   <si>
@@ -433,6 +487,9 @@
   </si>
   <si>
     <t>Eishalle Asiago;HEAD;HEAD;BASSO;MANTOVANI</t>
+  </si>
+  <si>
+    <t>Eishalle Cortina;MOSCHEN;PINIE;MANTOVANI;Ricco</t>
   </si>
 </sst>
 </file>
@@ -750,7 +807,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:BO56"/>
+  <dimension ref="A3:BR56"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="J9" sqref="J9"/>
@@ -827,7 +884,7 @@
     <col min="71" max="71" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="15" customHeight="1" spans="1:67" x14ac:dyDescent="0.25">
+    <row r="3" ht="15" customHeight="1" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1026,723 +1083,891 @@
       <c r="BN3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="4" ht="15" customHeight="1" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="BO3" t="s">
+        <v>66</v>
+      </c>
+      <c r="BP3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="I4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="K4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="L4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="M4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="N4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="O4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="P4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="Q4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="R4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="S4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="T4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="U4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="V4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="W4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="X4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="Y4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="Z4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="AA4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="AB4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="AC4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="AD4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="AE4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="AF4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="AG4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="AH4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="AI4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>72</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>70</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>70</v>
+      </c>
+      <c r="BB4" t="s">
+        <v>70</v>
+      </c>
+      <c r="BC4" t="s">
+        <v>70</v>
+      </c>
+      <c r="BD4" t="s">
+        <v>73</v>
+      </c>
+      <c r="BE4" t="s">
+        <v>73</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>73</v>
+      </c>
+      <c r="BG4" t="s">
+        <v>73</v>
+      </c>
+      <c r="BH4" t="s">
+        <v>73</v>
+      </c>
+      <c r="BI4" t="s">
+        <v>73</v>
+      </c>
+      <c r="BJ4" t="s">
+        <v>75</v>
+      </c>
+      <c r="BK4" t="s">
+        <v>75</v>
+      </c>
+      <c r="BL4" t="s">
+        <v>76</v>
+      </c>
+      <c r="BM4" t="s">
+        <v>76</v>
+      </c>
+      <c r="BN4" t="s">
+        <v>76</v>
+      </c>
+      <c r="BO4" t="s">
+        <v>77</v>
+      </c>
+      <c r="BP4" t="s">
+        <v>77</v>
+      </c>
+      <c r="BQ4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" t="s">
+        <v>71</v>
+      </c>
+      <c r="I5" t="s">
+        <v>71</v>
+      </c>
+      <c r="J5" t="s">
+        <v>71</v>
+      </c>
+      <c r="K5" t="s">
+        <v>71</v>
+      </c>
+      <c r="L5" t="s">
+        <v>72</v>
+      </c>
+      <c r="M5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O5" t="s">
+        <v>71</v>
+      </c>
+      <c r="P5" t="s">
         <v>69</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="Q5" t="s">
+        <v>71</v>
+      </c>
+      <c r="R5" t="s">
+        <v>71</v>
+      </c>
+      <c r="S5" t="s">
+        <v>71</v>
+      </c>
+      <c r="T5" t="s">
+        <v>71</v>
+      </c>
+      <c r="U5" t="s">
+        <v>71</v>
+      </c>
+      <c r="V5" t="s">
+        <v>71</v>
+      </c>
+      <c r="W5" t="s">
+        <v>71</v>
+      </c>
+      <c r="X5" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>77</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>76</v>
+      </c>
+      <c r="BB5" t="s">
+        <v>82</v>
+      </c>
+      <c r="BC5" t="s">
+        <v>76</v>
+      </c>
+      <c r="BD5" t="s">
+        <v>81</v>
+      </c>
+      <c r="BE5" t="s">
+        <v>77</v>
+      </c>
+      <c r="BG5" t="s">
+        <v>77</v>
+      </c>
+      <c r="BH5" t="s">
+        <v>77</v>
+      </c>
+      <c r="BI5" t="s">
+        <v>83</v>
+      </c>
+      <c r="BJ5" t="s">
+        <v>80</v>
+      </c>
+      <c r="BK5" t="s">
+        <v>78</v>
+      </c>
+      <c r="BN5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1" spans="1:66" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J6" t="s">
+        <v>72</v>
+      </c>
+      <c r="K6" t="s">
+        <v>72</v>
+      </c>
+      <c r="L6" t="s">
+        <v>71</v>
+      </c>
+      <c r="N6" t="s">
+        <v>76</v>
+      </c>
+      <c r="O6" t="s">
+        <v>72</v>
+      </c>
+      <c r="P6" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>70</v>
+      </c>
+      <c r="R6" t="s">
+        <v>72</v>
+      </c>
+      <c r="T6" t="s">
+        <v>70</v>
+      </c>
+      <c r="U6" t="s">
+        <v>74</v>
+      </c>
+      <c r="W6" t="s">
+        <v>73</v>
+      </c>
+      <c r="X6" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB6" t="s">
         <v>69</v>
       </c>
-      <c r="AK4" t="s">
+      <c r="AC6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>76</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>78</v>
+      </c>
+      <c r="BB6" t="s">
+        <v>85</v>
+      </c>
+      <c r="BC6" t="s">
+        <v>86</v>
+      </c>
+      <c r="BI6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1" spans="2:61" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I7" t="s">
+        <v>76</v>
+      </c>
+      <c r="J7" t="s">
+        <v>73</v>
+      </c>
+      <c r="L7" t="s">
+        <v>70</v>
+      </c>
+      <c r="N7" t="s">
+        <v>85</v>
+      </c>
+      <c r="O7" t="s">
+        <v>71</v>
+      </c>
+      <c r="P7" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>73</v>
+      </c>
+      <c r="R7" t="s">
+        <v>70</v>
+      </c>
+      <c r="T7" t="s">
+        <v>73</v>
+      </c>
+      <c r="U7" t="s">
+        <v>73</v>
+      </c>
+      <c r="W7" t="s">
+        <v>75</v>
+      </c>
+      <c r="X7" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA7" t="s">
         <v>69</v>
       </c>
-      <c r="AL4" t="s">
+      <c r="AB7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC7" t="s">
         <v>69</v>
       </c>
-      <c r="AM4" t="s">
+      <c r="AD7" t="s">
         <v>69</v>
       </c>
-      <c r="AN4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AQ4" t="s">
+      <c r="AF7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB7" t="s">
+        <v>79</v>
+      </c>
+      <c r="BC7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" t="s">
+        <v>77</v>
+      </c>
+      <c r="J8" t="s">
+        <v>76</v>
+      </c>
+      <c r="L8" t="s">
+        <v>75</v>
+      </c>
+      <c r="N8" t="s">
+        <v>84</v>
+      </c>
+      <c r="O8" t="s">
         <v>70</v>
       </c>
-      <c r="AR4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AS4" t="s">
-        <v>71</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>67</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>67</v>
-      </c>
-      <c r="AV4" t="s">
-        <v>67</v>
-      </c>
-      <c r="AW4" t="s">
-        <v>67</v>
-      </c>
-      <c r="AX4" t="s">
-        <v>67</v>
-      </c>
-      <c r="AY4" t="s">
-        <v>67</v>
-      </c>
-      <c r="AZ4" t="s">
-        <v>67</v>
-      </c>
-      <c r="BA4" t="s">
-        <v>67</v>
-      </c>
-      <c r="BB4" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC4" t="s">
-        <v>67</v>
-      </c>
-      <c r="BD4" t="s">
+      <c r="P8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>83</v>
+      </c>
+      <c r="R8" t="s">
+        <v>73</v>
+      </c>
+      <c r="T8" t="s">
+        <v>75</v>
+      </c>
+      <c r="U8" t="s">
+        <v>77</v>
+      </c>
+      <c r="W8" t="s">
+        <v>79</v>
+      </c>
+      <c r="X8" t="s">
         <v>70</v>
       </c>
-      <c r="BE4" t="s">
+      <c r="Y8" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>73</v>
+      </c>
+      <c r="AS8" t="s">
+        <v>87</v>
+      </c>
+      <c r="BB8" t="s">
+        <v>81</v>
+      </c>
+      <c r="BC8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" ht="15" customHeight="1" spans="2:55" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G9" t="s">
+        <v>79</v>
+      </c>
+      <c r="J9" t="s">
+        <v>77</v>
+      </c>
+      <c r="L9" t="s">
+        <v>76</v>
+      </c>
+      <c r="N9" t="s">
+        <v>81</v>
+      </c>
+      <c r="O9" t="s">
+        <v>84</v>
+      </c>
+      <c r="P9" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>77</v>
+      </c>
+      <c r="R9" t="s">
+        <v>75</v>
+      </c>
+      <c r="W9" t="s">
+        <v>81</v>
+      </c>
+      <c r="X9" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>83</v>
+      </c>
+      <c r="BB9" t="s">
+        <v>77</v>
+      </c>
+      <c r="BC9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" ht="15" customHeight="1" spans="6:55" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" t="s">
+        <v>81</v>
+      </c>
+      <c r="L10" t="s">
+        <v>85</v>
+      </c>
+      <c r="N10" t="s">
+        <v>77</v>
+      </c>
+      <c r="O10" t="s">
+        <v>81</v>
+      </c>
+      <c r="P10" t="s">
+        <v>74</v>
+      </c>
+      <c r="W10" t="s">
+        <v>77</v>
+      </c>
+      <c r="X10" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>76</v>
+      </c>
+      <c r="BC10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" ht="15" customHeight="1" spans="6:55" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>79</v>
+      </c>
+      <c r="O11" t="s">
+        <v>77</v>
+      </c>
+      <c r="P11" t="s">
         <v>70</v>
       </c>
-      <c r="BF4" t="s">
-        <v>70</v>
-      </c>
-      <c r="BG4" t="s">
-        <v>70</v>
-      </c>
-      <c r="BH4" t="s">
-        <v>70</v>
-      </c>
-      <c r="BI4" t="s">
-        <v>70</v>
-      </c>
-      <c r="BJ4" t="s">
-        <v>72</v>
-      </c>
-      <c r="BK4" t="s">
-        <v>72</v>
-      </c>
-      <c r="BL4" t="s">
+      <c r="X11" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" ht="15" customHeight="1" spans="12:34" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>81</v>
+      </c>
+      <c r="P12" t="s">
         <v>73</v>
       </c>
-      <c r="BM4" t="s">
-        <v>73</v>
-      </c>
-      <c r="BN4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" ht="15" customHeight="1" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G5" t="s">
-        <v>67</v>
-      </c>
-      <c r="H5" t="s">
-        <v>68</v>
-      </c>
-      <c r="I5" t="s">
-        <v>68</v>
-      </c>
-      <c r="J5" t="s">
-        <v>68</v>
-      </c>
-      <c r="K5" t="s">
-        <v>68</v>
-      </c>
-      <c r="L5" t="s">
-        <v>69</v>
-      </c>
-      <c r="M5" t="s">
-        <v>69</v>
-      </c>
-      <c r="N5" t="s">
-        <v>72</v>
-      </c>
-      <c r="O5" t="s">
-        <v>68</v>
-      </c>
-      <c r="P5" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>68</v>
-      </c>
-      <c r="R5" t="s">
-        <v>68</v>
-      </c>
-      <c r="S5" t="s">
-        <v>68</v>
-      </c>
-      <c r="T5" t="s">
-        <v>68</v>
-      </c>
-      <c r="U5" t="s">
-        <v>68</v>
-      </c>
-      <c r="V5" t="s">
-        <v>68</v>
-      </c>
-      <c r="W5" t="s">
-        <v>68</v>
-      </c>
-      <c r="X5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>74</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>69</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>69</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>70</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>70</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>70</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>70</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>72</v>
-      </c>
-      <c r="AP5" t="s">
-        <v>70</v>
-      </c>
-      <c r="AQ5" t="s">
+      <c r="X12" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>85</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" ht="15" customHeight="1" spans="12:34" x14ac:dyDescent="0.25">
+      <c r="L13" t="s">
+        <v>77</v>
+      </c>
+      <c r="P13" t="s">
+        <v>83</v>
+      </c>
+      <c r="X13" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" ht="15" customHeight="1" spans="12:26" x14ac:dyDescent="0.25">
+      <c r="P14" t="s">
         <v>75</v>
       </c>
-      <c r="AR5" t="s">
-        <v>69</v>
-      </c>
-      <c r="AS5" t="s">
-        <v>70</v>
-      </c>
-      <c r="AT5" t="s">
-        <v>72</v>
-      </c>
-      <c r="AU5" t="s">
-        <v>76</v>
-      </c>
-      <c r="AV5" t="s">
-        <v>74</v>
-      </c>
-      <c r="AW5" t="s">
-        <v>76</v>
-      </c>
-      <c r="AX5" t="s">
-        <v>73</v>
-      </c>
-      <c r="BA5" t="s">
-        <v>73</v>
-      </c>
-      <c r="BB5" t="s">
+      <c r="X14" t="s">
         <v>77</v>
       </c>
-      <c r="BC5" t="s">
-        <v>73</v>
-      </c>
-      <c r="BI5" t="s">
-        <v>78</v>
-      </c>
-      <c r="BJ5" t="s">
-        <v>76</v>
-      </c>
-      <c r="BK5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" ht="15" customHeight="1" spans="1:63" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F6" t="s">
-        <v>72</v>
-      </c>
-      <c r="G6" t="s">
-        <v>72</v>
-      </c>
-      <c r="H6" t="s">
-        <v>69</v>
-      </c>
-      <c r="I6" t="s">
-        <v>69</v>
-      </c>
-      <c r="J6" t="s">
-        <v>69</v>
-      </c>
-      <c r="K6" t="s">
-        <v>69</v>
-      </c>
-      <c r="L6" t="s">
-        <v>68</v>
-      </c>
-      <c r="N6" t="s">
-        <v>73</v>
-      </c>
-      <c r="O6" t="s">
-        <v>69</v>
-      </c>
-      <c r="P6" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>67</v>
-      </c>
-      <c r="R6" t="s">
-        <v>69</v>
-      </c>
-      <c r="T6" t="s">
-        <v>67</v>
-      </c>
-      <c r="U6" t="s">
-        <v>71</v>
-      </c>
-      <c r="W6" t="s">
-        <v>70</v>
-      </c>
-      <c r="X6" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>69</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE6" t="s">
+      <c r="Z14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" ht="15" customHeight="1" spans="16:26" x14ac:dyDescent="0.25">
+      <c r="P15" t="s">
         <v>77</v>
       </c>
-      <c r="AF6" t="s">
-        <v>73</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>69</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>73</v>
-      </c>
-      <c r="AS6" t="s">
-        <v>72</v>
-      </c>
-      <c r="AT6" t="s">
-        <v>74</v>
-      </c>
-      <c r="BB6" t="s">
-        <v>80</v>
-      </c>
-      <c r="BC6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" ht="15" customHeight="1" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F7" t="s">
-        <v>73</v>
-      </c>
-      <c r="G7" t="s">
-        <v>73</v>
-      </c>
-      <c r="H7" t="s">
-        <v>70</v>
-      </c>
-      <c r="I7" t="s">
-        <v>73</v>
-      </c>
-      <c r="J7" t="s">
-        <v>70</v>
-      </c>
-      <c r="L7" t="s">
-        <v>67</v>
-      </c>
-      <c r="N7" t="s">
-        <v>80</v>
-      </c>
-      <c r="O7" t="s">
-        <v>68</v>
-      </c>
-      <c r="P7" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>70</v>
-      </c>
-      <c r="R7" t="s">
-        <v>67</v>
-      </c>
-      <c r="T7" t="s">
-        <v>70</v>
-      </c>
-      <c r="U7" t="s">
-        <v>70</v>
-      </c>
-      <c r="W7" t="s">
-        <v>72</v>
-      </c>
-      <c r="X7" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>66</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>71</v>
-      </c>
-      <c r="AT7" t="s">
-        <v>76</v>
-      </c>
-      <c r="BB7" t="s">
-        <v>75</v>
-      </c>
-      <c r="BC7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" ht="15" customHeight="1" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="F8" t="s">
-        <v>80</v>
-      </c>
-      <c r="G8" t="s">
-        <v>80</v>
-      </c>
-      <c r="J8" t="s">
-        <v>73</v>
-      </c>
-      <c r="L8" t="s">
-        <v>72</v>
-      </c>
-      <c r="N8" t="s">
-        <v>79</v>
-      </c>
-      <c r="O8" t="s">
-        <v>67</v>
-      </c>
-      <c r="P8" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>78</v>
-      </c>
-      <c r="R8" t="s">
-        <v>70</v>
-      </c>
-      <c r="T8" t="s">
-        <v>72</v>
-      </c>
-      <c r="W8" t="s">
-        <v>75</v>
-      </c>
-      <c r="X8" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>79</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>70</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>81</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>70</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>70</v>
-      </c>
-      <c r="BC8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" ht="15" customHeight="1" spans="6:55" x14ac:dyDescent="0.25">
-      <c r="F9" t="s">
-        <v>79</v>
-      </c>
-      <c r="G9" t="s">
-        <v>75</v>
-      </c>
-      <c r="L9" t="s">
-        <v>73</v>
-      </c>
-      <c r="O9" t="s">
-        <v>79</v>
-      </c>
-      <c r="P9" t="s">
-        <v>69</v>
-      </c>
-      <c r="R9" t="s">
-        <v>72</v>
-      </c>
-      <c r="X9" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>73</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>75</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>70</v>
-      </c>
-      <c r="AH9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" ht="15" customHeight="1" spans="6:34" x14ac:dyDescent="0.25">
-      <c r="L10" t="s">
-        <v>80</v>
-      </c>
-      <c r="P10" t="s">
-        <v>71</v>
-      </c>
-      <c r="X10" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>73</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>80</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" ht="15" customHeight="1" spans="12:34" x14ac:dyDescent="0.25">
-      <c r="L11" t="s">
-        <v>75</v>
-      </c>
-      <c r="P11" t="s">
-        <v>67</v>
-      </c>
-      <c r="X11" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>81</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" ht="15" customHeight="1" spans="12:27" x14ac:dyDescent="0.25">
-      <c r="P12" t="s">
-        <v>70</v>
-      </c>
-      <c r="X12" t="s">
-        <v>79</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" ht="15" customHeight="1" spans="16:26" x14ac:dyDescent="0.25">
-      <c r="P13" t="s">
-        <v>78</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" ht="15" customHeight="1" spans="16:26" x14ac:dyDescent="0.25">
-      <c r="P14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" ht="15" customHeight="1" spans="16:16" x14ac:dyDescent="0.25"/>
-    <row r="16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="16" ht="15" customHeight="1" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" ht="15" customHeight="1" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" ht="15" customHeight="1" spans="16:16" x14ac:dyDescent="0.25"/>
     <row r="21" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1787,7 +2012,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:O42"/>
+  <dimension ref="A3:R42"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="N4" sqref="N4"/>
@@ -1811,54 +2036,63 @@
     <col min="15" max="15" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="15" customHeight="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" ht="15" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K3" t="s">
         <v>78</v>
       </c>
-      <c r="H3" t="s">
-        <v>72</v>
-      </c>
-      <c r="I3" t="s">
-        <v>73</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M3" t="s">
+        <v>84</v>
+      </c>
+      <c r="N3" t="s">
+        <v>79</v>
+      </c>
+      <c r="O3" t="s">
+        <v>80</v>
+      </c>
+      <c r="P3" t="s">
         <v>81</v>
       </c>
-      <c r="K3" t="s">
-        <v>74</v>
-      </c>
-      <c r="L3" t="s">
-        <v>80</v>
-      </c>
-      <c r="M3" t="s">
-        <v>79</v>
-      </c>
-      <c r="N3" t="s">
-        <v>75</v>
-      </c>
-      <c r="O3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" ht="15" customHeight="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q3" t="s">
+        <v>77</v>
+      </c>
+      <c r="R3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1904,8 +2138,17 @@
       <c r="O4" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" ht="15" customHeight="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>34</v>
+      </c>
+      <c r="R4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1951,8 +2194,17 @@
       <c r="O5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" ht="15" customHeight="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>1</v>
+      </c>
+      <c r="R5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1998,8 +2250,17 @@
       <c r="O6" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="7" ht="15" customHeight="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>56</v>
+      </c>
+      <c r="R6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -2045,8 +2306,17 @@
       <c r="O7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="8" ht="15" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P7" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>51</v>
+      </c>
+      <c r="R7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2077,8 +2347,14 @@
       <c r="N8" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="9" ht="15" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P8" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -2109,8 +2385,14 @@
       <c r="N9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" ht="15" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P9" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -2141,8 +2423,14 @@
       <c r="N10" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="11" ht="15" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P10" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -2173,8 +2461,14 @@
       <c r="N11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" ht="15" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P11" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -2196,8 +2490,14 @@
       <c r="I12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="P12" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -2219,8 +2519,14 @@
       <c r="I13" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="14" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="P13" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -2242,8 +2548,14 @@
       <c r="I14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="P14" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -2265,8 +2577,14 @@
       <c r="I15" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="P15" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -2288,8 +2606,14 @@
       <c r="I16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="P16" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -2311,8 +2635,14 @@
       <c r="I17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="P17" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -2334,8 +2664,14 @@
       <c r="I18" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="P18" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -2357,8 +2693,14 @@
       <c r="I19" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="P19" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -2377,8 +2719,11 @@
       <c r="I20" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -2397,8 +2742,11 @@
       <c r="I21" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="22" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -2417,8 +2765,11 @@
       <c r="I22" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="23" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Q22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -2437,8 +2788,11 @@
       <c r="I23" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="24" ht="15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -2454,8 +2808,11 @@
       <c r="F24" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="25" ht="15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -2471,8 +2828,11 @@
       <c r="F25" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" ht="15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -2488,8 +2848,11 @@
       <c r="F26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="27" ht="15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -2505,8 +2868,11 @@
       <c r="F27" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="28" ht="15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -2519,8 +2885,11 @@
       <c r="F28" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="29" ht="15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -2533,8 +2902,11 @@
       <c r="F29" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" ht="15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -2547,8 +2919,11 @@
       <c r="F30" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="31" ht="15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="Q30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>25</v>
       </c>
@@ -2561,8 +2936,11 @@
       <c r="F31" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="32" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="Q31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -2572,8 +2950,11 @@
       <c r="C32" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="33" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="Q32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>27</v>
       </c>
@@ -2583,8 +2964,11 @@
       <c r="C33" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="34" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="Q33" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -2594,8 +2978,11 @@
       <c r="C34" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="35" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="Q34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -2605,8 +2992,11 @@
       <c r="C35" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="36" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="Q35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" ht="15" customHeight="1" spans="17:17" x14ac:dyDescent="0.25"/>
     <row r="37" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="38" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2620,7 +3010,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:O13"/>
+  <dimension ref="A3:R13"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="96" zoomScaleNormal="130">
       <selection activeCell="N4" sqref="N4"/>
@@ -2687,241 +3077,289 @@
     <col min="63" max="63" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="15" customHeight="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" ht="15" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="G3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K3" t="s">
         <v>78</v>
       </c>
-      <c r="H3" t="s">
-        <v>72</v>
-      </c>
-      <c r="I3" t="s">
-        <v>73</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
+        <v>85</v>
+      </c>
+      <c r="M3" t="s">
+        <v>84</v>
+      </c>
+      <c r="N3" t="s">
+        <v>79</v>
+      </c>
+      <c r="O3" t="s">
+        <v>80</v>
+      </c>
+      <c r="P3" t="s">
         <v>81</v>
       </c>
-      <c r="K3" t="s">
-        <v>74</v>
-      </c>
-      <c r="L3" t="s">
-        <v>80</v>
-      </c>
-      <c r="M3" t="s">
-        <v>79</v>
-      </c>
-      <c r="N3" t="s">
-        <v>75</v>
-      </c>
-      <c r="O3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" ht="15" customHeight="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q3" t="s">
+        <v>77</v>
+      </c>
+      <c r="R3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="F4" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="G4" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="H4" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="I4" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="J4" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="K4" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="L4" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="M4" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="N4" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="O4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" ht="15" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="P4" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>104</v>
+      </c>
+      <c r="R4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="C5" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="F5" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="H5" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="I5" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="L5" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="M5" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="N5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" ht="15" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="P5" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="C6" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="E6" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="F6" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="H6" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="I6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="P6" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="C7" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="E7" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="F7" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="H7" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="I7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" ht="15" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="P7" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="B8" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="C8" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="E8" t="s">
-        <v>124</v>
+        <v>139</v>
       </c>
       <c r="F8" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="I8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" ht="15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="C9" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="E9" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="F9" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="10" ht="15" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="B10" t="s">
-        <v>133</v>
+        <v>150</v>
       </c>
       <c r="C10" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="F10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="11" ht="15" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" ht="15" customHeight="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="B11" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="C11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>156</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" ht="15" customHeight="1" spans="17:17" x14ac:dyDescent="0.25"/>
     <row r="13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
git popravljene odpadne tekme
</commit_message>
<xml_diff>
--- a/data/AHLdelegacije.xlsx
+++ b/data/AHLdelegacije.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
   </bookViews>
   <sheets>
     <sheet sheetId="1" name="AHL" state="visible" r:id="rId4"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="231">
   <si>
     <t>BULOVEC</t>
   </si>
@@ -651,9 +651,6 @@
     <t>Eishalle Ritten;EGGER;LAZZERI;BEDANA;SLAVIERO</t>
   </si>
   <si>
-    <t>Eishalle Cortina;PINIE;STEFENELLI;CRISTELI;DE ZORDO</t>
-  </si>
-  <si>
     <t>Eishalle Asiago;MOSCHEN;PINIE;CRISTELI;SLAVIERO</t>
   </si>
   <si>
@@ -682,9 +679,6 @@
   </si>
   <si>
     <t>Eishalle Canazei;BENVEGNU;PINIE;CARRITO;PIRAS</t>
-  </si>
-  <si>
-    <t>Eishalle Canazei;EGGER;LEGA;BEDANA;SLAVIERO</t>
   </si>
   <si>
     <t>Eishalle Gröden;BENVEGNU;LAZZERI;BEDANA;DE ZORDO</t>
@@ -1035,7 +1029,7 @@
   <dimension ref="A3:BU56"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="AB13" sqref="AB13"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" customHeight="1"/>
@@ -2194,7 +2188,7 @@
         <v>82</v>
       </c>
       <c r="AQ8" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="AS8" t="s">
         <v>80</v>
@@ -2331,7 +2325,7 @@
         <v>90</v>
       </c>
       <c r="AQ9" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="AS9" t="s">
         <v>82</v>
@@ -2425,9 +2419,6 @@
       <c r="AP10" t="s">
         <v>80</v>
       </c>
-      <c r="AQ10" t="s">
-        <v>97</v>
-      </c>
       <c r="AS10" t="s">
         <v>109</v>
       </c>
@@ -2559,7 +2550,7 @@
         <v>110</v>
       </c>
       <c r="W12" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="X12" t="s">
         <v>91</v>
@@ -2586,7 +2577,7 @@
         <v>110</v>
       </c>
       <c r="BB12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="BC12" t="s">
         <v>82</v>
@@ -2624,7 +2615,7 @@
         <v>104</v>
       </c>
       <c r="W13" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="X13" t="s">
         <v>100</v>
@@ -2643,9 +2634,6 @@
       </c>
       <c r="AH13" t="s">
         <v>82</v>
-      </c>
-      <c r="BB13" t="s">
-        <v>93</v>
       </c>
       <c r="BC13" t="s">
         <v>89</v>
@@ -2656,7 +2644,7 @@
         <v>93</v>
       </c>
       <c r="F14" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G14" t="s">
         <v>82</v>
@@ -2676,9 +2664,6 @@
       <c r="Q14" t="s">
         <v>110</v>
       </c>
-      <c r="W14" t="s">
-        <v>104</v>
-      </c>
       <c r="X14" t="s">
         <v>81</v>
       </c>
@@ -2692,7 +2677,7 @@
         <v>92</v>
       </c>
       <c r="AB14" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AH14" t="s">
         <v>109</v>
@@ -2703,7 +2688,7 @@
     </row>
     <row r="15" ht="15" customHeight="1" spans="5:55" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G15" t="s">
         <v>95</v>
@@ -2736,7 +2721,7 @@
         <v>100</v>
       </c>
       <c r="AB15" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="AH15" t="s">
         <v>80</v>
@@ -2746,9 +2731,6 @@
       </c>
     </row>
     <row r="16" ht="15" customHeight="1" spans="6:55" x14ac:dyDescent="0.25">
-      <c r="F16" t="s">
-        <v>93</v>
-      </c>
       <c r="G16" t="s">
         <v>97</v>
       </c>
@@ -2756,7 +2738,7 @@
         <v>96</v>
       </c>
       <c r="N16" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="O16" t="s">
         <v>95</v>
@@ -2771,7 +2753,7 @@
         <v>94</v>
       </c>
       <c r="Y16" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="Z16" t="s">
         <v>80</v>
@@ -2779,9 +2761,6 @@
       <c r="AA16" t="s">
         <v>82</v>
       </c>
-      <c r="AB16" t="s">
-        <v>93</v>
-      </c>
       <c r="AH16" t="s">
         <v>80</v>
       </c>
@@ -2789,7 +2768,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" ht="15" customHeight="1" spans="6:55" x14ac:dyDescent="0.25">
+    <row r="17" ht="15" customHeight="1" spans="7:55" x14ac:dyDescent="0.25">
       <c r="G17" t="s">
         <v>93</v>
       </c>
@@ -2797,7 +2776,7 @@
         <v>95</v>
       </c>
       <c r="N17" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="O17" t="s">
         <v>97</v>
@@ -2809,7 +2788,7 @@
         <v>82</v>
       </c>
       <c r="Y17" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="Z17" t="s">
         <v>94</v>
@@ -2829,7 +2808,7 @@
         <v>93</v>
       </c>
       <c r="N18" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="O18" t="s">
         <v>93</v>
@@ -2840,9 +2819,6 @@
       <c r="X18" t="s">
         <v>95</v>
       </c>
-      <c r="Y18" t="s">
-        <v>93</v>
-      </c>
       <c r="Z18" t="s">
         <v>80</v>
       </c>
@@ -2854,9 +2830,6 @@
       </c>
     </row>
     <row r="19" ht="15" customHeight="1" spans="12:34" x14ac:dyDescent="0.25">
-      <c r="N19" t="s">
-        <v>104</v>
-      </c>
       <c r="P19" t="s">
         <v>94</v>
       </c>
@@ -2873,7 +2846,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" ht="15" customHeight="1" spans="14:34" x14ac:dyDescent="0.25">
+    <row r="20" ht="15" customHeight="1" spans="16:34" x14ac:dyDescent="0.25">
       <c r="P20" t="s">
         <v>82</v>
       </c>
@@ -2881,7 +2854,7 @@
         <v>93</v>
       </c>
       <c r="Z20" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AA20" t="s">
         <v>97</v>
@@ -2895,7 +2868,7 @@
         <v>82</v>
       </c>
       <c r="Z21" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="AA21" t="s">
         <v>104</v>
@@ -2905,11 +2878,8 @@
       <c r="P22" t="s">
         <v>105</v>
       </c>
-      <c r="Z22" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="23" ht="15" customHeight="1" spans="16:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" ht="15" customHeight="1" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P23" t="s">
         <v>105</v>
       </c>
@@ -2982,7 +2952,7 @@
   <dimension ref="A3:AL42"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="W12" sqref="W12"/>
+      <selection activeCell="AE20" sqref="AE20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" customHeight="1"/>
@@ -3007,6 +2977,7 @@
     <col min="22" max="22" width="20.28515625" customWidth="1"/>
     <col min="23" max="23" width="15.85546875" customWidth="1"/>
     <col min="25" max="25" width="30.42578125" customWidth="1"/>
+    <col min="31" max="31" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" ht="15" customHeight="1" spans="1:38" x14ac:dyDescent="0.25">
@@ -4313,9 +4284,6 @@
       <c r="Y20" t="s">
         <v>53</v>
       </c>
-      <c r="AE20" t="s">
-        <v>27</v>
-      </c>
       <c r="AG20" t="s">
         <v>23</v>
       </c>
@@ -4351,9 +4319,6 @@
       <c r="Y21" t="s">
         <v>26</v>
       </c>
-      <c r="AE21" t="s">
-        <v>5</v>
-      </c>
       <c r="AG21" t="s">
         <v>27</v>
       </c>
@@ -4389,9 +4354,6 @@
       <c r="Y22" t="s">
         <v>24</v>
       </c>
-      <c r="AE22" t="s">
-        <v>13</v>
-      </c>
       <c r="AG22" t="s">
         <v>13</v>
       </c>
@@ -4427,9 +4389,6 @@
       <c r="Y23" t="s">
         <v>42</v>
       </c>
-      <c r="AE23" t="s">
-        <v>25</v>
-      </c>
       <c r="AG23" t="s">
         <v>42</v>
       </c>
@@ -4462,9 +4421,6 @@
       <c r="Y24" t="s">
         <v>4</v>
       </c>
-      <c r="AE24" t="s">
-        <v>53</v>
-      </c>
       <c r="AG24" t="s">
         <v>4</v>
       </c>
@@ -4494,9 +4450,6 @@
       <c r="Y25" t="s">
         <v>27</v>
       </c>
-      <c r="AE25" t="s">
-        <v>22</v>
-      </c>
       <c r="AG25" t="s">
         <v>26</v>
       </c>
@@ -4526,9 +4479,6 @@
       <c r="Y26" t="s">
         <v>71</v>
       </c>
-      <c r="AE26" t="s">
-        <v>24</v>
-      </c>
       <c r="AG26" t="s">
         <v>24</v>
       </c>
@@ -4557,9 +4507,6 @@
       </c>
       <c r="Y27" t="s">
         <v>6</v>
-      </c>
-      <c r="AE27" t="s">
-        <v>42</v>
       </c>
       <c r="AG27" t="s">
         <v>25</v>
@@ -4706,7 +4653,7 @@
   <dimension ref="A3:AL13"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="96" zoomScaleNormal="130">
-      <selection activeCell="W6" sqref="W6"/>
+      <selection activeCell="AE15" sqref="AE15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" customHeight="1"/>
@@ -5205,77 +5152,71 @@
       <c r="Y8" t="s">
         <v>210</v>
       </c>
-      <c r="AE8" t="s">
+      <c r="AG8" t="s">
         <v>211</v>
       </c>
-      <c r="AG8" t="s">
+      <c r="AI8" t="s">
         <v>212</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="9" ht="15" customHeight="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>213</v>
+      </c>
+      <c r="B9" t="s">
         <v>214</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>215</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>216</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>217</v>
       </c>
-      <c r="F9" t="s">
+      <c r="Q9" t="s">
         <v>218</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="V9" t="s">
         <v>219</v>
       </c>
-      <c r="V9" t="s">
+      <c r="Y9" t="s">
         <v>220</v>
       </c>
-      <c r="Y9" t="s">
+      <c r="AG9" t="s">
         <v>221</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>222</v>
-      </c>
-      <c r="AG9" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>222</v>
+      </c>
+      <c r="B10" t="s">
+        <v>223</v>
+      </c>
+      <c r="C10" t="s">
         <v>224</v>
       </c>
-      <c r="B10" t="s">
+      <c r="F10" t="s">
         <v>225</v>
       </c>
-      <c r="C10" t="s">
+      <c r="Y10" t="s">
         <v>226</v>
-      </c>
-      <c r="F10" t="s">
-        <v>227</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>227</v>
+      </c>
+      <c r="B11" t="s">
+        <v>228</v>
+      </c>
+      <c r="C11" t="s">
         <v>229</v>
       </c>
-      <c r="B11" t="s">
+      <c r="Y11" t="s">
         <v>230</v>
-      </c>
-      <c r="C11" t="s">
-        <v>231</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
2.1. po koncu dneva
</commit_message>
<xml_diff>
--- a/data/AHLdelegacije.xlsx
+++ b/data/AHLdelegacije.xlsx
@@ -1,22 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54CAEFE-8379-4833-A0BD-BC68B1BC3CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="AHL" state="visible" r:id="rId4"/>
-    <sheet sheetId="3" name="AHL_DAT" state="visible" r:id="rId5"/>
-    <sheet sheetId="4" name="AHL_DAT_STRING" state="visible" r:id="rId6"/>
+    <sheet name="AHL" sheetId="1" r:id="rId1"/>
+    <sheet name="AHL_DAT" sheetId="3" r:id="rId2"/>
+    <sheet name="AHL_DAT_STRING" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2633" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2631" uniqueCount="416">
   <si>
     <t>FAJDIGA</t>
   </si>
@@ -441,42 +453,42 @@
     <t>zbrisano</t>
   </si>
   <si>
+    <t>2021-12-27</t>
+  </si>
+  <si>
+    <t>2021-12-23</t>
+  </si>
+  <si>
+    <t>Zbrisano</t>
+  </si>
+  <si>
+    <t>2021-12-21</t>
+  </si>
+  <si>
+    <t>2021-12-15</t>
+  </si>
+  <si>
+    <t>2021-12-29</t>
+  </si>
+  <si>
+    <t>2021-12-01</t>
+  </si>
+  <si>
+    <t>2022-01-05</t>
+  </si>
+  <si>
+    <t>2022-01-03</t>
+  </si>
+  <si>
+    <t>2021-12-18</t>
+  </si>
+  <si>
+    <t>2022-01-18</t>
+  </si>
+  <si>
     <t>2022-01-02</t>
   </si>
   <si>
-    <t>2021-12-27</t>
-  </si>
-  <si>
-    <t>2021-12-23</t>
-  </si>
-  <si>
-    <t>Zbrisano</t>
-  </si>
-  <si>
-    <t>2021-12-21</t>
-  </si>
-  <si>
-    <t>2021-12-15</t>
-  </si>
-  <si>
-    <t>2021-12-29</t>
-  </si>
-  <si>
-    <t>2021-12-01</t>
-  </si>
-  <si>
-    <t>2022-01-05</t>
-  </si>
-  <si>
-    <t>2022-01-03</t>
-  </si>
-  <si>
-    <t>2021-12-18</t>
-  </si>
-  <si>
-    <t>2022-01-18</t>
-  </si>
-  <si>
     <t>2022-01-11</t>
   </si>
   <si>
@@ -837,7 +849,7 @@
     <t>Eishalle Lustenau;HUBER;LEHNER;HUBER;MOIDL</t>
   </si>
   <si>
-    <t>Eishalle Ritten;GIACOMOZZI;KUMMER;CRISTELI;HOLZER</t>
+    <t>Eishalle Ritten;GIACOMOZZI;VIRTA;CRISTELI;PACE</t>
   </si>
   <si>
     <t>Eisarena Salzburg;FAJDIGA;WIDMANN;KAINBERGER;KANYO</t>
@@ -951,7 +963,7 @@
     <t>Eishalle Sterzing;EGGER;HOLZER;EISL;RINKER</t>
   </si>
   <si>
-    <t>Eishalle Gröden;MOSCHEN;PINIE;DE ZORDO;PACE</t>
+    <t>Eishalle Cortina;EGGER;SORAPERRA;BRONDI;PIRAS</t>
   </si>
   <si>
     <t>Eishalle Zell am See;DURCHNER;HEINRICHER;LEGAT;VOICAN</t>
@@ -1048,9 +1060,6 @@
   </si>
   <si>
     <t>Eishalle Asiago;LESNIAK;PODLESNIK;PUFF;SNOJ</t>
-  </si>
-  <si>
-    <t>Eishalle Cortina;EGGER;SORAPERRA;BRONDI;PIRAS</t>
   </si>
   <si>
     <t>Sportpark Kitzbühel;LEHNER;WUNTSCHEK;MATTHEY;PUFF</t>
@@ -1272,22 +1281,22 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="238"/>
-      <color rgb="FF006100"/>
-      <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1299,7 +1308,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.1499984740745262"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1636,14 +1645,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:BW56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:BV56"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.140625" customWidth="1"/>
@@ -1714,10 +1723,10 @@
     <col min="72" max="72" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" ht="14.45" customHeight="1" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:74" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>COUNTIF(A4:A39,"&lt;&gt;")</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <f t="shared" ref="B2:E2" si="0">COUNTIF(B4:B40,"&lt;&gt;")</f>
@@ -1725,19 +1734,19 @@
       </c>
       <c r="C2">
         <f>COUNTIF(C4:C39,"&lt;&gt;")</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <f>COUNTIF(F4:F39,"&lt;&gt;")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2">
         <f>COUNTIF(G4:G38,"&lt;&gt;")</f>
@@ -1745,39 +1754,39 @@
       </c>
       <c r="H2">
         <f>COUNTIF(H4:H38,"&lt;&gt;")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I2">
         <f>COUNTIF(I4:I39,"&lt;&gt;")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J2">
         <f>COUNTIF(J4:J39,"&lt;&gt;")</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K2">
         <f>COUNTIF(K4:K40,"&lt;&gt;")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L2">
         <f>COUNTIF(L4:L39,"&lt;&gt;")</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M2">
         <f>COUNTIF(M4:M39,"&lt;&gt;")</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N2">
         <f>COUNTIF(N4:N36,"&lt;&gt;")</f>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="O2">
         <f>COUNTIF(O4:O38,"&lt;&gt;")</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P2">
         <f>COUNTIF(P4:P39,"&lt;&gt;")</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q2">
         <f>COUNTIF(Q4:Q34,"&lt;&gt;")</f>
@@ -1785,35 +1794,35 @@
       </c>
       <c r="R2">
         <f>COUNTIF(R4:R40,"&lt;&gt;")</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="S2">
         <f>COUNTIF(S4:S39,"&lt;&gt;")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="T2">
         <f>COUNTIF(T4:T40,"&lt;&gt;")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="U2">
         <f>COUNTIF(U4:U36,"&lt;&gt;")</f>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="V2">
         <f>COUNTIF(V4:V38,"&lt;&gt;")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="W2">
         <f>COUNTIF(W4:W39,"&lt;&gt;")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="X2">
         <f>COUNTIF(X4:X39,"&lt;&gt;")</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="Y2">
         <f>COUNTIF(Y4:Y40,"&lt;&gt;")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Z2">
         <f>COUNTIF(Z4:Z39,"&lt;&gt;")</f>
@@ -1821,75 +1830,75 @@
       </c>
       <c r="AA2">
         <f>COUNTIF(AA4:AA39,"&lt;&gt;")</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AB2">
         <f>COUNTIF(AB4:AB37,"&lt;&gt;")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AC2">
         <f>COUNTIF(AC4:AC38,"&lt;&gt;")</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AD2">
         <f>COUNTIF(AD4:AD38,"&lt;&gt;")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AE2">
         <f>COUNTIF(AE4:AE37,"&lt;&gt;")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AF2">
         <f>COUNTIF(AF4:AF39,"&lt;&gt;")</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AG2">
         <f>COUNTIF(AG4:AG39,"&lt;&gt;")</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AH2">
         <f>COUNTIF(AH4:AH40,"&lt;&gt;")</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AI2">
         <f>COUNTIF(AI4:AI35,"&lt;&gt;")</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AJ2">
         <f>COUNTIF(AJ4:AJ39,"&lt;&gt;")</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AK2">
         <f>COUNTIF(AK4:AK37,"&lt;&gt;")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AL2">
         <f>COUNTIF(AL4:AL40,"&lt;&gt;")</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AM2">
         <f>COUNTIF(AM4:AM40,"&lt;&gt;")</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AN2">
         <f>COUNTIF(AN4:AN38,"&lt;&gt;")</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AO2">
         <f>COUNTIF(AO4:AO38,"&lt;&gt;")</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AP2">
         <f>COUNTIF(AP4:AP39,"&lt;&gt;")</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AQ2">
         <f>COUNTIF(AQ4:AQ37,"&lt;&gt;")</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AR2">
         <f>COUNTIF(AR4:AR37,"&lt;&gt;")</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AS2">
         <f>COUNTIF(AS4:AS38,"&lt;&gt;")</f>
@@ -1897,23 +1906,23 @@
       </c>
       <c r="AT2">
         <f>COUNTIF(AT4:AT39,"&lt;&gt;")</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AU2">
         <f>COUNTIF(AU4:AU36,"&lt;&gt;")</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AV2">
         <f>COUNTIF(AV4:AV38,"&lt;&gt;")</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AW2">
         <f>COUNTIF(AW4:AW36,"&lt;&gt;")</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AX2">
         <f>COUNTIF(AX4:AX38,"&lt;&gt;")</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AY2">
         <f>COUNTIF(AY4:AY40,"&lt;&gt;")</f>
@@ -1921,43 +1930,43 @@
       </c>
       <c r="AZ2">
         <f>COUNTIF(AZ4:AZ39,"&lt;&gt;")</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="BA2">
         <f>COUNTIF(BA4:BA37,"&lt;&gt;")</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="BB2">
         <f>COUNTIF(BB4:BB31,"&lt;&gt;")</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="BC2">
         <f>COUNTIF(BC4:BC36,"&lt;&gt;")</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="BD2">
         <f>COUNTIF(BD4:BD35,"&lt;&gt;")</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="BE2">
         <f>COUNTIF(BE4:BE38,"&lt;&gt;")</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="BF2">
         <f>COUNTIF(BF4:BF35,"&lt;&gt;")</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="BG2">
         <f>COUNTIF(BG4:BG37,"&lt;&gt;")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="BH2">
         <f>COUNTIF(BH4:BH36,"&lt;&gt;")</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="BI2">
         <f>COUNTIF(BI4:BI37,"&lt;&gt;")</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="BJ2">
         <f>COUNTIF(BJ4:BJ40,"&lt;&gt;")</f>
@@ -1969,15 +1978,15 @@
       </c>
       <c r="BL2">
         <f>COUNTIF(BL4:BL38,"&lt;&gt;")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BM2">
         <f>COUNTIF(BM4:BM38,"&lt;&gt;")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="BN2">
         <f>COUNTIF(BN4:BN37,"&lt;&gt;")</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="BO2">
         <f>COUNTIF(BO4:BO40,"&lt;&gt;")</f>
@@ -2000,7 +2009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2224,7 +2233,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -2448,7 +2457,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" ht="15" customHeight="1" spans="1:74" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -2660,7 +2669,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" ht="15" customHeight="1" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>82</v>
       </c>
@@ -2863,7 +2872,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" ht="15" customHeight="1" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>93</v>
       </c>
@@ -3066,7 +3075,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" ht="15" customHeight="1" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>85</v>
       </c>
@@ -3263,7 +3272,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" ht="15" customHeight="1" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>101</v>
       </c>
@@ -3457,7 +3466,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" ht="15" customHeight="1" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>96</v>
       </c>
@@ -3651,7 +3660,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" ht="15" customHeight="1" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>120</v>
       </c>
@@ -3836,7 +3845,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" ht="15" customHeight="1" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>116</v>
       </c>
@@ -4021,7 +4030,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" ht="15" customHeight="1" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>105</v>
       </c>
@@ -4191,7 +4200,7 @@
         <v>120</v>
       </c>
       <c r="BI13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="BK13" t="s">
         <v>104</v>
@@ -4203,15 +4212,15 @@
         <v>105</v>
       </c>
       <c r="BN13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
-    <row r="14" ht="15" customHeight="1" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>131</v>
@@ -4229,7 +4238,7 @@
         <v>90</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>105</v>
@@ -4278,13 +4287,13 @@
         <v>114</v>
       </c>
       <c r="AB14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC14" t="s">
         <v>103</v>
       </c>
       <c r="AD14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AF14" t="s">
         <v>105</v>
@@ -4353,7 +4362,7 @@
         <v>97</v>
       </c>
       <c r="BD14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="BE14" t="s">
         <v>104</v>
@@ -4362,7 +4371,7 @@
         <v>90</v>
       </c>
       <c r="BG14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BH14" t="s">
         <v>88</v>
@@ -4377,13 +4386,13 @@
         <v>89</v>
       </c>
       <c r="BM14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="BN14" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="15" ht="15" customHeight="1" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>129</v>
       </c>
@@ -4391,7 +4400,7 @@
         <v>140</v>
       </c>
       <c r="D15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>125</v>
@@ -4409,7 +4418,7 @@
         <v>126</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K15" t="s">
         <v>105</v>
@@ -4421,7 +4430,7 @@
         <v>120</v>
       </c>
       <c r="N15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O15" t="s">
         <v>107</v>
@@ -4520,7 +4529,7 @@
         <v>120</v>
       </c>
       <c r="BA15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="BB15" t="s">
         <v>128</v>
@@ -4532,7 +4541,7 @@
         <v>89</v>
       </c>
       <c r="BE15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="BF15" t="s">
         <v>129</v>
@@ -4553,13 +4562,13 @@
         <v>90</v>
       </c>
       <c r="BM15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="BN15" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="16" ht="15" customHeight="1" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:74" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>90</v>
       </c>
@@ -4570,10 +4579,10 @@
         <v>91</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>126</v>
@@ -4621,7 +4630,7 @@
         <v>91</v>
       </c>
       <c r="AB16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC16" t="s">
         <v>134</v>
@@ -4633,7 +4642,7 @@
         <v>140</v>
       </c>
       <c r="AG16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AH16" t="s">
         <v>140</v>
@@ -4663,7 +4672,7 @@
         <v>103</v>
       </c>
       <c r="AR16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AS16" t="s">
         <v>116</v>
@@ -4678,7 +4687,7 @@
         <v>102</v>
       </c>
       <c r="AW16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AX16" t="s">
         <v>114</v>
@@ -4710,8 +4719,11 @@
       <c r="BH16" t="s">
         <v>128</v>
       </c>
+      <c r="BI16" t="s">
+        <v>140</v>
+      </c>
       <c r="BK16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="BL16" t="s">
         <v>129</v>
@@ -4723,9 +4735,9 @@
         <v>129</v>
       </c>
     </row>
-    <row r="17" ht="15" customHeight="1" spans="1:66" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D17" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>137</v>
@@ -4785,7 +4797,7 @@
         <v>91</v>
       </c>
       <c r="AD17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AF17" t="s">
         <v>128</v>
@@ -4809,7 +4821,7 @@
         <v>88</v>
       </c>
       <c r="AN17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AO17" t="s">
         <v>124</v>
@@ -4827,7 +4839,7 @@
         <v>128</v>
       </c>
       <c r="AT17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AU17" t="s">
         <v>128</v>
@@ -4845,7 +4857,7 @@
         <v>116</v>
       </c>
       <c r="BA17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BB17" t="s">
         <v>129</v>
@@ -4857,16 +4869,19 @@
         <v>125</v>
       </c>
       <c r="BE17" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="BG17" t="s">
         <v>122</v>
       </c>
       <c r="BH17" t="s">
-        <v>146</v>
+        <v>145</v>
+      </c>
+      <c r="BI17" t="s">
+        <v>152</v>
       </c>
       <c r="BK17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BL17" t="s">
         <v>126</v>
@@ -4875,10 +4890,10 @@
         <v>126</v>
       </c>
       <c r="BN17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
-    <row r="18" ht="15" customHeight="1" spans="4:66" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D18" s="5" t="s">
         <v>137</v>
       </c>
@@ -4887,7 +4902,7 @@
       </c>
       <c r="G18" s="2"/>
       <c r="L18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M18" t="s">
         <v>121</v>
@@ -4896,7 +4911,7 @@
         <v>91</v>
       </c>
       <c r="O18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="P18" t="s">
         <v>97</v>
@@ -4911,7 +4926,7 @@
         <v>126</v>
       </c>
       <c r="X18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Z18" t="s">
         <v>109</v>
@@ -4929,7 +4944,7 @@
         <v>140</v>
       </c>
       <c r="AG18" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="AH18" t="s">
         <v>128</v>
@@ -4959,13 +4974,13 @@
         <v>120</v>
       </c>
       <c r="AR18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AS18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AT18" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="AU18" t="s">
         <v>139</v>
@@ -4992,11 +5007,14 @@
         <v>105</v>
       </c>
       <c r="BD18" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="BE18" t="s">
         <v>137</v>
       </c>
+      <c r="BG18" t="s">
+        <v>152</v>
+      </c>
       <c r="BH18" t="s">
         <v>129</v>
       </c>
@@ -5007,7 +5025,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="19" ht="15" customHeight="1" spans="4:66" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D19" s="2" t="s">
         <v>126</v>
       </c>
@@ -5027,7 +5045,7 @@
         <v>124</v>
       </c>
       <c r="X19" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="Z19" t="s">
         <v>102</v>
@@ -5036,7 +5054,7 @@
         <v>126</v>
       </c>
       <c r="AC19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AF19" t="s">
         <v>122</v>
@@ -5045,7 +5063,7 @@
         <v>105</v>
       </c>
       <c r="AH19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AI19" t="s">
         <v>136</v>
@@ -5054,13 +5072,13 @@
         <v>137</v>
       </c>
       <c r="AL19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AM19" t="s">
         <v>124</v>
       </c>
       <c r="AN19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AO19" t="s">
         <v>90</v>
@@ -5075,7 +5093,7 @@
         <v>139</v>
       </c>
       <c r="AS19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="AT19" t="s">
         <v>140</v>
@@ -5102,7 +5120,7 @@
         <v>125</v>
       </c>
       <c r="BC19" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="BE19" t="s">
         <v>125</v>
@@ -5114,9 +5132,9 @@
         <v>140</v>
       </c>
     </row>
-    <row r="20" ht="15" customHeight="1" spans="4:63" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M20" t="s">
         <v>124</v>
@@ -5149,16 +5167,16 @@
         <v>128</v>
       </c>
       <c r="AJ20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="AL20" t="s">
         <v>140</v>
       </c>
       <c r="AM20" t="s">
+        <v>144</v>
+      </c>
+      <c r="AN20" t="s">
         <v>145</v>
-      </c>
-      <c r="AN20" t="s">
-        <v>146</v>
       </c>
       <c r="AO20" t="s">
         <v>126</v>
@@ -5176,7 +5194,7 @@
         <v>126</v>
       </c>
       <c r="AU20" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="AV20" t="s">
         <v>97</v>
@@ -5191,7 +5209,7 @@
         <v>140</v>
       </c>
       <c r="BA20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="BC20" t="s">
         <v>140</v>
@@ -5203,15 +5221,15 @@
         <v>140</v>
       </c>
     </row>
-    <row r="21" ht="15" customHeight="1" spans="12:63" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L21" t="s">
         <v>129</v>
       </c>
       <c r="M21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N21" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="O21" s="2" t="s">
         <v>126</v>
@@ -5229,13 +5247,13 @@
         <v>140</v>
       </c>
       <c r="AI21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AL21" t="s">
+        <v>152</v>
+      </c>
+      <c r="AM21" t="s">
         <v>141</v>
-      </c>
-      <c r="AM21" t="s">
-        <v>142</v>
       </c>
       <c r="AN21" t="s">
         <v>91</v>
@@ -5262,7 +5280,7 @@
         <v>120</v>
       </c>
       <c r="AX21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AZ21" t="s">
         <v>129</v>
@@ -5271,10 +5289,10 @@
         <v>125</v>
       </c>
       <c r="BC21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
-    <row r="22" ht="15" customHeight="1" spans="12:55" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L22" s="2" t="s">
         <v>126</v>
       </c>
@@ -5306,7 +5324,7 @@
         <v>129</v>
       </c>
       <c r="AQ22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AS22" t="s">
         <v>140</v>
@@ -5327,7 +5345,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="23" ht="15" customHeight="1" spans="12:55" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M23" t="s">
         <v>90</v>
       </c>
@@ -5341,10 +5359,10 @@
         <v>118</v>
       </c>
       <c r="AI23" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="AL23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AM23" t="s">
         <v>125</v>
@@ -5365,7 +5383,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="24" ht="15" customHeight="1" spans="13:55" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M24" t="s">
         <v>129</v>
       </c>
@@ -5379,7 +5397,7 @@
         <v>107</v>
       </c>
       <c r="AI24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AL24" t="s">
         <v>125</v>
@@ -5394,7 +5412,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="25" ht="15" customHeight="1" spans="13:50" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M25" s="2" t="s">
         <v>125</v>
       </c>
@@ -5402,10 +5420,10 @@
         <v>107</v>
       </c>
       <c r="AI25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AQ25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AV25" t="s">
         <v>105</v>
@@ -5414,7 +5432,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="26" ht="15.75" customHeight="1" spans="13:50" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z26" t="s">
         <v>108</v>
       </c>
@@ -5428,7 +5446,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="27" ht="15" customHeight="1" spans="26:48" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z27" t="s">
         <v>87</v>
       </c>
@@ -5442,15 +5460,15 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" ht="15" customHeight="1" spans="26:48" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z28" t="s">
         <v>97</v>
       </c>
       <c r="AV28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
-    <row r="29" ht="15" customHeight="1" spans="26:48" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z29" t="s">
         <v>97</v>
       </c>
@@ -5458,15 +5476,15 @@
         <v>129</v>
       </c>
     </row>
-    <row r="30" ht="15" customHeight="1" spans="26:48" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z30" t="s">
         <v>114</v>
       </c>
       <c r="AV30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
-    <row r="31" ht="15" customHeight="1" spans="26:48" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z31" t="s">
         <v>114</v>
       </c>
@@ -5474,15 +5492,15 @@
         <v>139</v>
       </c>
     </row>
-    <row r="32" ht="15" customHeight="1" spans="26:48" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:66" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AV32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
-    <row r="33" ht="15" customHeight="1" spans="26:48" x14ac:dyDescent="0.25">
+    <row r="33" spans="26:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z33" t="s">
         <v>88</v>
       </c>
@@ -5490,112 +5508,112 @@
         <v>125</v>
       </c>
     </row>
-    <row r="34" ht="15" customHeight="1" spans="26:48" x14ac:dyDescent="0.25">
+    <row r="34" spans="26:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z34" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="35" ht="15" customHeight="1" spans="26:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="26:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z35" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="36" ht="15" customHeight="1" spans="26:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="26:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z36" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="37" ht="15" customHeight="1" spans="26:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="26:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z37" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="38" ht="15" customHeight="1" spans="26:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="26:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
-    <row r="39" ht="15" customHeight="1" spans="26:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="26:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z39" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="40" ht="15" customHeight="1" spans="26:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="26:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z40" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="41" ht="15" customHeight="1" spans="26:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="26:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z41" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="42" ht="15" customHeight="1" spans="26:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="26:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z42" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="43" ht="15" customHeight="1" spans="26:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="26:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z43" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
-    <row r="44" ht="15" customHeight="1" spans="26:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="26:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z44" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="45" ht="15" customHeight="1" spans="26:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="26:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z45" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
-    <row r="46" ht="15" customHeight="1" spans="26:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="26:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z46" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
-    <row r="47" ht="15" customHeight="1" spans="26:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="26:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
-    <row r="48" ht="15" customHeight="1" spans="26:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="26:48" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z48" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="49" ht="15" customHeight="1" spans="26:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="26:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z49" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="50" ht="15" customHeight="1" spans="26:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="26:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z50" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="51" ht="15" customHeight="1" spans="26:26" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="26:26" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="26:26" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="26:26" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="26:26" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="26:26" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="26:26" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:BZ42"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="BR11" sqref="BR11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BP26" sqref="BP26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
@@ -5643,7 +5661,7 @@
     <col min="88" max="88" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -5780,7 +5798,7 @@
         <v>104</v>
       </c>
       <c r="AT3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AU3" t="s">
         <v>88</v>
@@ -5807,22 +5825,22 @@
         <v>105</v>
       </c>
       <c r="BC3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="BD3" t="s">
         <v>132</v>
       </c>
       <c r="BE3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="BF3" t="s">
         <v>134</v>
       </c>
       <c r="BG3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="BH3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BI3" t="s">
         <v>139</v>
@@ -5834,28 +5852,28 @@
         <v>153</v>
       </c>
       <c r="BL3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="BM3" t="s">
         <v>89</v>
       </c>
       <c r="BN3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="BO3" t="s">
         <v>91</v>
       </c>
       <c r="BP3" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="BQ3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="BR3" t="s">
         <v>122</v>
       </c>
       <c r="BS3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="BT3" t="s">
         <v>90</v>
@@ -5870,7 +5888,7 @@
         <v>135</v>
       </c>
       <c r="BX3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="BY3" t="s">
         <v>126</v>
@@ -5879,7 +5897,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -6115,7 +6133,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -6351,7 +6369,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -6587,7 +6605,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -6823,7 +6841,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -6966,7 +6984,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -7091,7 +7109,7 @@
         <v>65</v>
       </c>
       <c r="BP9" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="BT9" t="s">
         <v>63</v>
@@ -7109,7 +7127,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -7252,7 +7270,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -7377,7 +7395,7 @@
         <v>28</v>
       </c>
       <c r="BP11" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="BT11" t="s">
         <v>72</v>
@@ -7395,7 +7413,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -7493,7 +7511,7 @@
         <v>54</v>
       </c>
       <c r="BP12" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="BT12" t="s">
         <v>57</v>
@@ -7508,7 +7526,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -7606,7 +7624,7 @@
         <v>25</v>
       </c>
       <c r="BP13" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="BT13" t="s">
         <v>40</v>
@@ -7621,7 +7639,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -7719,7 +7737,7 @@
         <v>52</v>
       </c>
       <c r="BP14" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="BT14" t="s">
         <v>22</v>
@@ -7734,7 +7752,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -7832,7 +7850,7 @@
         <v>39</v>
       </c>
       <c r="BP15" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="BT15" t="s">
         <v>41</v>
@@ -7847,7 +7865,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -7932,9 +7950,6 @@
       <c r="BO16" t="s">
         <v>4</v>
       </c>
-      <c r="BP16" t="s">
-        <v>54</v>
-      </c>
       <c r="BT16" t="s">
         <v>65</v>
       </c>
@@ -7948,7 +7963,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -8033,9 +8048,6 @@
       <c r="BO17" t="s">
         <v>24</v>
       </c>
-      <c r="BP17" t="s">
-        <v>32</v>
-      </c>
       <c r="BT17" t="s">
         <v>38</v>
       </c>
@@ -8049,7 +8061,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -8134,9 +8146,6 @@
       <c r="BO18" t="s">
         <v>14</v>
       </c>
-      <c r="BP18" t="s">
-        <v>55</v>
-      </c>
       <c r="BT18" t="s">
         <v>29</v>
       </c>
@@ -8150,7 +8159,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -8235,9 +8244,6 @@
       <c r="BO19" t="s">
         <v>5</v>
       </c>
-      <c r="BP19" t="s">
-        <v>45</v>
-      </c>
       <c r="BT19" t="s">
         <v>14</v>
       </c>
@@ -8251,7 +8257,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -8340,7 +8346,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -8429,7 +8435,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -8518,7 +8524,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -8607,7 +8613,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -8678,7 +8684,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -8749,7 +8755,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>44</v>
       </c>
@@ -8820,7 +8826,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -8891,7 +8897,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>46</v>
       </c>
@@ -8923,7 +8929,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -8955,7 +8961,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -8987,7 +8993,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -9019,7 +9025,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -9039,7 +9045,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -9059,7 +9065,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -9079,7 +9085,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>28</v>
       </c>
@@ -9099,43 +9105,43 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="37" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="39" ht="15" customHeight="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="40" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A3:BZ13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="96" zoomScaleNormal="96">
-      <selection activeCell="BP22" sqref="BP22"/>
+    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="BP6" sqref="BP6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="79" customWidth="1"/>
     <col min="2" max="2" width="46.42578125" customWidth="1"/>
@@ -9217,7 +9223,7 @@
     <col min="88" max="88" width="49.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>44450</v>
       </c>
@@ -9354,7 +9360,7 @@
         <v>104</v>
       </c>
       <c r="AT3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AU3" t="s">
         <v>88</v>
@@ -9381,22 +9387,22 @@
         <v>105</v>
       </c>
       <c r="BC3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="BD3" t="s">
         <v>132</v>
       </c>
       <c r="BE3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="BF3" t="s">
         <v>134</v>
       </c>
       <c r="BG3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="BH3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BI3" t="s">
         <v>139</v>
@@ -9408,28 +9414,28 @@
         <v>153</v>
       </c>
       <c r="BL3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="BM3" t="s">
         <v>89</v>
       </c>
       <c r="BN3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="BO3" t="s">
         <v>91</v>
       </c>
       <c r="BP3" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="BQ3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="BR3" t="s">
         <v>122</v>
       </c>
       <c r="BS3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="BT3" t="s">
         <v>90</v>
@@ -9444,7 +9450,7 @@
         <v>135</v>
       </c>
       <c r="BX3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="BY3" t="s">
         <v>126</v>
@@ -9453,7 +9459,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>154</v>
       </c>
@@ -9689,7 +9695,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="5" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>232</v>
       </c>
@@ -9832,7 +9838,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="6" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>279</v>
       </c>
@@ -9945,7 +9951,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="7" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>316</v>
       </c>
@@ -10030,238 +10036,235 @@
       <c r="BO7" t="s">
         <v>343</v>
       </c>
-      <c r="BP7" s="7" t="s">
+      <c r="BT7" t="s">
         <v>344</v>
       </c>
-      <c r="BT7" t="s">
+      <c r="BV7" t="s">
         <v>345</v>
       </c>
-      <c r="BV7" t="s">
+      <c r="BY7" t="s">
         <v>346</v>
       </c>
-      <c r="BY7" t="s">
+      <c r="BZ7" t="s">
         <v>347</v>
       </c>
-      <c r="BZ7" t="s">
+    </row>
+    <row r="8" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>348</v>
       </c>
+      <c r="C8" t="s">
+        <v>349</v>
+      </c>
+      <c r="D8" t="s">
+        <v>350</v>
+      </c>
+      <c r="E8" t="s">
+        <v>351</v>
+      </c>
+      <c r="G8" t="s">
+        <v>352</v>
+      </c>
+      <c r="H8" t="s">
+        <v>353</v>
+      </c>
+      <c r="K8" t="s">
+        <v>354</v>
+      </c>
+      <c r="O8" t="s">
+        <v>355</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>356</v>
+      </c>
+      <c r="S8" t="s">
+        <v>357</v>
+      </c>
+      <c r="U8" t="s">
+        <v>358</v>
+      </c>
+      <c r="X8" t="s">
+        <v>359</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>360</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>361</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>362</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>363</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>364</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>365</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>366</v>
+      </c>
+      <c r="AQ8" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="AS8" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="AU8" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="AV8" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="BB8" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="BM8" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="BO8" t="s">
+        <v>373</v>
+      </c>
+      <c r="BV8" t="s">
+        <v>374</v>
+      </c>
+      <c r="BY8" t="s">
+        <v>375</v>
+      </c>
+      <c r="BZ8" t="s">
+        <v>376</v>
+      </c>
     </row>
-    <row r="8" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>349</v>
-      </c>
-      <c r="C8" t="s">
-        <v>350</v>
-      </c>
-      <c r="D8" t="s">
-        <v>351</v>
-      </c>
-      <c r="E8" t="s">
-        <v>352</v>
-      </c>
-      <c r="G8" t="s">
-        <v>353</v>
-      </c>
-      <c r="H8" t="s">
-        <v>354</v>
-      </c>
-      <c r="K8" t="s">
-        <v>355</v>
-      </c>
-      <c r="O8" t="s">
-        <v>356</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>357</v>
-      </c>
-      <c r="S8" t="s">
-        <v>358</v>
-      </c>
-      <c r="U8" t="s">
-        <v>359</v>
-      </c>
-      <c r="X8" t="s">
-        <v>360</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>361</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>362</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>363</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>364</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>365</v>
-      </c>
-      <c r="AM8" t="s">
-        <v>366</v>
-      </c>
-      <c r="AO8" t="s">
-        <v>367</v>
-      </c>
-      <c r="AQ8" s="7" t="s">
-        <v>368</v>
-      </c>
-      <c r="AS8" s="7" t="s">
-        <v>369</v>
-      </c>
-      <c r="AU8" s="7" t="s">
-        <v>370</v>
-      </c>
-      <c r="AV8" s="7" t="s">
-        <v>371</v>
-      </c>
-      <c r="BB8" s="7" t="s">
-        <v>372</v>
-      </c>
-      <c r="BM8" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="BO8" t="s">
-        <v>374</v>
-      </c>
-      <c r="BV8" t="s">
-        <v>375</v>
-      </c>
-      <c r="BY8" t="s">
-        <v>376</v>
-      </c>
-      <c r="BZ8" t="s">
+    <row r="9" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>377</v>
       </c>
+      <c r="D9" t="s">
+        <v>378</v>
+      </c>
+      <c r="E9" t="s">
+        <v>379</v>
+      </c>
+      <c r="G9" t="s">
+        <v>380</v>
+      </c>
+      <c r="K9" t="s">
+        <v>381</v>
+      </c>
+      <c r="O9" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>383</v>
+      </c>
+      <c r="S9" t="s">
+        <v>384</v>
+      </c>
+      <c r="U9" t="s">
+        <v>385</v>
+      </c>
+      <c r="X9" t="s">
+        <v>386</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>387</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>388</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>389</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>390</v>
+      </c>
+      <c r="AO9" t="s">
+        <v>391</v>
+      </c>
+      <c r="AS9" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="AU9" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="AV9" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="BB9" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="BM9" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="BV9" t="s">
+        <v>397</v>
+      </c>
+      <c r="BY9" t="s">
+        <v>398</v>
+      </c>
+      <c r="BZ9" t="s">
+        <v>399</v>
+      </c>
     </row>
-    <row r="9" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>378</v>
-      </c>
-      <c r="D9" t="s">
-        <v>379</v>
-      </c>
-      <c r="E9" t="s">
-        <v>380</v>
-      </c>
-      <c r="G9" t="s">
-        <v>381</v>
-      </c>
-      <c r="K9" t="s">
-        <v>382</v>
-      </c>
-      <c r="O9" t="s">
-        <v>383</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>384</v>
-      </c>
-      <c r="S9" t="s">
-        <v>385</v>
-      </c>
-      <c r="U9" t="s">
-        <v>386</v>
-      </c>
-      <c r="X9" t="s">
-        <v>387</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>388</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>389</v>
-      </c>
-      <c r="AI9" t="s">
-        <v>390</v>
-      </c>
-      <c r="AM9" t="s">
-        <v>391</v>
-      </c>
-      <c r="AO9" t="s">
-        <v>392</v>
-      </c>
-      <c r="AS9" s="7" t="s">
-        <v>393</v>
-      </c>
-      <c r="AU9" s="7" t="s">
-        <v>394</v>
-      </c>
-      <c r="AV9" s="7" t="s">
-        <v>395</v>
-      </c>
-      <c r="BB9" s="7" t="s">
-        <v>396</v>
-      </c>
-      <c r="BM9" s="7" t="s">
-        <v>397</v>
-      </c>
-      <c r="BV9" t="s">
-        <v>398</v>
-      </c>
-      <c r="BY9" t="s">
-        <v>399</v>
-      </c>
-      <c r="BZ9" t="s">
+    <row r="10" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>400</v>
       </c>
+      <c r="D10" t="s">
+        <v>401</v>
+      </c>
+      <c r="E10" t="s">
+        <v>402</v>
+      </c>
+      <c r="K10" t="s">
+        <v>403</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>404</v>
+      </c>
+      <c r="AS10" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="BB10" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="BV10" t="s">
+        <v>407</v>
+      </c>
+      <c r="BY10" t="s">
+        <v>408</v>
+      </c>
+      <c r="BZ10" t="s">
+        <v>409</v>
+      </c>
     </row>
-    <row r="10" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>401</v>
-      </c>
-      <c r="D10" t="s">
-        <v>402</v>
-      </c>
-      <c r="E10" t="s">
-        <v>403</v>
-      </c>
-      <c r="K10" t="s">
-        <v>404</v>
-      </c>
-      <c r="AI10" t="s">
-        <v>405</v>
-      </c>
-      <c r="AS10" s="7" t="s">
-        <v>406</v>
-      </c>
-      <c r="BB10" s="7" t="s">
-        <v>407</v>
-      </c>
-      <c r="BV10" t="s">
-        <v>408</v>
-      </c>
-      <c r="BY10" t="s">
-        <v>409</v>
-      </c>
-      <c r="BZ10" t="s">
+    <row r="11" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>410</v>
       </c>
+      <c r="D11" t="s">
+        <v>411</v>
+      </c>
+      <c r="K11" t="s">
+        <v>412</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>413</v>
+      </c>
+      <c r="BY11" t="s">
+        <v>414</v>
+      </c>
+      <c r="BZ11" t="s">
+        <v>415</v>
+      </c>
     </row>
-    <row r="11" ht="15" customHeight="1" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>411</v>
-      </c>
-      <c r="D11" t="s">
-        <v>412</v>
-      </c>
-      <c r="K11" t="s">
-        <v>413</v>
-      </c>
-      <c r="AI11" t="s">
-        <v>414</v>
-      </c>
-      <c r="BY11" t="s">
-        <v>415</v>
-      </c>
-      <c r="BZ11" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="12" ht="15" customHeight="1" spans="77:78" x14ac:dyDescent="0.25"/>
-    <row r="13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>